<commit_message>
Add missing modified date to xlsx file in inbox
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat\inbox-excel-vocabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371F10F6-626D-49B8-882A-181B872F8812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F349B219-9781-4BD8-8C16-2BAE13950E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="2340" windowWidth="28785" windowHeight="12915" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="806">
   <si>
     <t>Template version</t>
   </si>
@@ -3222,14 +3222,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3789,65 +3789,65 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -3946,61 +3946,61 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
@@ -4064,391 +4064,391 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
     </row>
     <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="5"/>
@@ -4461,1096 +4461,1096 @@
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
     </row>
     <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
     </row>
     <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
     </row>
     <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="28"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
     </row>
     <row r="56" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="28"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
     </row>
     <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="28"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="29"/>
     </row>
     <row r="58" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="28"/>
-      <c r="J58" s="28"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="29"/>
     </row>
     <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-      <c r="J59" s="28"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="29"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="28"/>
-      <c r="J60" s="28"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="28"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
     </row>
     <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
-      <c r="J62" s="28"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
     </row>
     <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-      <c r="J63" s="28"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="28"/>
-      <c r="H64" s="28"/>
-      <c r="I64" s="28"/>
-      <c r="J64" s="28"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
     </row>
     <row r="65" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="28"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="29"/>
     </row>
     <row r="66" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="28"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
     </row>
     <row r="67" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="29"/>
     </row>
     <row r="68" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="28"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="28"/>
-      <c r="J68" s="28"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
     </row>
     <row r="69" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="28"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="29"/>
     </row>
     <row r="72" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="28"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
     </row>
     <row r="73" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="29"/>
     </row>
     <row r="74" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="28"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="28"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
     </row>
     <row r="75" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="28"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
     </row>
     <row r="76" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="28"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="28"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="28"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
     </row>
     <row r="77" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="28"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="28"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
     </row>
     <row r="78" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="28"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="28"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="28"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="29"/>
     </row>
     <row r="79" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="28"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="28"/>
-      <c r="G79" s="28"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="29"/>
     </row>
     <row r="80" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="28"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
     </row>
     <row r="81" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="28"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="29"/>
     </row>
     <row r="82" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="28"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="28"/>
-      <c r="F82" s="28"/>
-      <c r="G82" s="28"/>
-      <c r="H82" s="28"/>
-      <c r="I82" s="28"/>
-      <c r="J82" s="28"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
+      <c r="J82" s="29"/>
     </row>
     <row r="83" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="28"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="28"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="28"/>
-      <c r="I83" s="28"/>
-      <c r="J83" s="28"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="29"/>
     </row>
     <row r="84" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="28"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="28"/>
-      <c r="F84" s="28"/>
-      <c r="G84" s="28"/>
-      <c r="H84" s="28"/>
-      <c r="I84" s="28"/>
-      <c r="J84" s="28"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="29"/>
     </row>
     <row r="85" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="28"/>
-      <c r="H85" s="28"/>
-      <c r="I85" s="28"/>
-      <c r="J85" s="28"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
     </row>
     <row r="86" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
     </row>
     <row r="87" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="28"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
-      <c r="J87" s="28"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
     </row>
     <row r="88" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="28"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="28"/>
-      <c r="H88" s="28"/>
-      <c r="I88" s="28"/>
-      <c r="J88" s="28"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
+      <c r="J88" s="29"/>
     </row>
     <row r="89" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="27" t="s">
+      <c r="B90" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="28"/>
-      <c r="I90" s="28"/>
-      <c r="J90" s="28"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
     </row>
     <row r="91" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="28"/>
-      <c r="H91" s="28"/>
-      <c r="I91" s="28"/>
-      <c r="J91" s="28"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
     </row>
     <row r="92" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
-      <c r="E92" s="28"/>
-      <c r="F92" s="28"/>
-      <c r="G92" s="28"/>
-      <c r="H92" s="28"/>
-      <c r="I92" s="28"/>
-      <c r="J92" s="28"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="29"/>
     </row>
     <row r="93" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="29"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
+      <c r="J93" s="29"/>
     </row>
     <row r="94" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
+      <c r="J94" s="29"/>
     </row>
     <row r="95" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="28"/>
-      <c r="H95" s="28"/>
-      <c r="I95" s="28"/>
-      <c r="J95" s="28"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
+      <c r="J95" s="29"/>
     </row>
     <row r="96" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
     </row>
     <row r="97" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="28"/>
-      <c r="G97" s="28"/>
-      <c r="H97" s="28"/>
-      <c r="I97" s="28"/>
-      <c r="J97" s="28"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
     </row>
     <row r="98" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="28"/>
-      <c r="I98" s="28"/>
-      <c r="J98" s="28"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="29"/>
+      <c r="I98" s="29"/>
+      <c r="J98" s="29"/>
     </row>
     <row r="99" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="28"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="28"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="28"/>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
+      <c r="G99" s="29"/>
+      <c r="H99" s="29"/>
+      <c r="I99" s="29"/>
+      <c r="J99" s="29"/>
     </row>
     <row r="100" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="29"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
     </row>
     <row r="101" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
     </row>
     <row r="102" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
-      <c r="H102" s="28"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="29"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="29"/>
     </row>
     <row r="103" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="28"/>
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
-      <c r="E103" s="28"/>
-      <c r="F103" s="28"/>
-      <c r="G103" s="28"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="29"/>
+      <c r="D103" s="29"/>
+      <c r="E103" s="29"/>
+      <c r="F103" s="29"/>
+      <c r="G103" s="29"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="29"/>
+      <c r="J103" s="29"/>
     </row>
     <row r="104" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="28"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="28"/>
-      <c r="H104" s="28"/>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="29"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="29"/>
+      <c r="J104" s="29"/>
     </row>
     <row r="105" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="28"/>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
-      <c r="E105" s="28"/>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
+      <c r="B105" s="29"/>
+      <c r="C105" s="29"/>
+      <c r="D105" s="29"/>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="29"/>
+      <c r="J105" s="29"/>
     </row>
     <row r="106" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="28"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="28"/>
-      <c r="F106" s="28"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="28"/>
-      <c r="I106" s="28"/>
-      <c r="J106" s="28"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
     </row>
     <row r="107" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
-      <c r="E107" s="28"/>
-      <c r="F107" s="28"/>
-      <c r="G107" s="28"/>
-      <c r="H107" s="28"/>
-      <c r="I107" s="28"/>
-      <c r="J107" s="28"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
     </row>
     <row r="108" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="28"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="28"/>
-      <c r="F108" s="28"/>
-      <c r="G108" s="28"/>
-      <c r="H108" s="28"/>
-      <c r="I108" s="28"/>
-      <c r="J108" s="28"/>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="29"/>
+      <c r="E108" s="29"/>
+      <c r="F108" s="29"/>
+      <c r="G108" s="29"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
+      <c r="J108" s="29"/>
     </row>
     <row r="109" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="28"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="28"/>
-      <c r="F109" s="28"/>
-      <c r="G109" s="28"/>
-      <c r="H109" s="28"/>
-      <c r="I109" s="28"/>
-      <c r="J109" s="28"/>
+      <c r="B109" s="29"/>
+      <c r="C109" s="29"/>
+      <c r="D109" s="29"/>
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+      <c r="G109" s="29"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="29"/>
+      <c r="J109" s="29"/>
     </row>
     <row r="110" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="28"/>
-      <c r="F110" s="28"/>
-      <c r="G110" s="28"/>
-      <c r="H110" s="28"/>
-      <c r="I110" s="28"/>
-      <c r="J110" s="28"/>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+      <c r="G110" s="29"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="29"/>
+      <c r="J110" s="29"/>
     </row>
     <row r="111" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="28"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
-      <c r="E111" s="28"/>
-      <c r="F111" s="28"/>
-      <c r="G111" s="28"/>
-      <c r="H111" s="28"/>
-      <c r="I111" s="28"/>
-      <c r="J111" s="28"/>
+      <c r="B111" s="29"/>
+      <c r="C111" s="29"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="29"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="29"/>
+      <c r="I111" s="29"/>
+      <c r="J111" s="29"/>
     </row>
     <row r="112" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28"/>
-      <c r="F112" s="28"/>
-      <c r="G112" s="28"/>
-      <c r="H112" s="28"/>
-      <c r="I112" s="28"/>
-      <c r="J112" s="28"/>
+      <c r="B112" s="29"/>
+      <c r="C112" s="29"/>
+      <c r="D112" s="29"/>
+      <c r="E112" s="29"/>
+      <c r="F112" s="29"/>
+      <c r="G112" s="29"/>
+      <c r="H112" s="29"/>
+      <c r="I112" s="29"/>
+      <c r="J112" s="29"/>
     </row>
     <row r="113" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
-      <c r="F113" s="28"/>
-      <c r="G113" s="28"/>
-      <c r="H113" s="28"/>
-      <c r="I113" s="28"/>
-      <c r="J113" s="28"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="J113" s="29"/>
     </row>
     <row r="114" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="28"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
-      <c r="E114" s="28"/>
-      <c r="F114" s="28"/>
-      <c r="G114" s="28"/>
-      <c r="H114" s="28"/>
-      <c r="I114" s="28"/>
-      <c r="J114" s="28"/>
+      <c r="B114" s="29"/>
+      <c r="C114" s="29"/>
+      <c r="D114" s="29"/>
+      <c r="E114" s="29"/>
+      <c r="F114" s="29"/>
+      <c r="G114" s="29"/>
+      <c r="H114" s="29"/>
+      <c r="I114" s="29"/>
+      <c r="J114" s="29"/>
     </row>
     <row r="115" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="28"/>
-      <c r="C115" s="28"/>
-      <c r="D115" s="28"/>
-      <c r="E115" s="28"/>
-      <c r="F115" s="28"/>
-      <c r="G115" s="28"/>
-      <c r="H115" s="28"/>
-      <c r="I115" s="28"/>
-      <c r="J115" s="28"/>
+      <c r="B115" s="29"/>
+      <c r="C115" s="29"/>
+      <c r="D115" s="29"/>
+      <c r="E115" s="29"/>
+      <c r="F115" s="29"/>
+      <c r="G115" s="29"/>
+      <c r="H115" s="29"/>
+      <c r="I115" s="29"/>
+      <c r="J115" s="29"/>
     </row>
     <row r="116" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="28"/>
-      <c r="G116" s="28"/>
-      <c r="H116" s="28"/>
-      <c r="I116" s="28"/>
-      <c r="J116" s="28"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
+      <c r="J116" s="29"/>
     </row>
     <row r="117" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="27" t="s">
+      <c r="B118" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C118" s="28"/>
-      <c r="D118" s="28"/>
-      <c r="E118" s="28"/>
-      <c r="F118" s="28"/>
-      <c r="G118" s="28"/>
-      <c r="H118" s="28"/>
-      <c r="I118" s="28"/>
-      <c r="J118" s="28"/>
+      <c r="C118" s="29"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
+      <c r="G118" s="29"/>
+      <c r="H118" s="29"/>
+      <c r="I118" s="29"/>
+      <c r="J118" s="29"/>
     </row>
     <row r="119" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="28"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="28"/>
-      <c r="E119" s="28"/>
-      <c r="F119" s="28"/>
-      <c r="G119" s="28"/>
-      <c r="H119" s="28"/>
-      <c r="I119" s="28"/>
-      <c r="J119" s="28"/>
+      <c r="B119" s="29"/>
+      <c r="C119" s="29"/>
+      <c r="D119" s="29"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="29"/>
+      <c r="G119" s="29"/>
+      <c r="H119" s="29"/>
+      <c r="I119" s="29"/>
+      <c r="J119" s="29"/>
     </row>
     <row r="120" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="28"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="28"/>
-      <c r="E120" s="28"/>
-      <c r="F120" s="28"/>
-      <c r="G120" s="28"/>
-      <c r="H120" s="28"/>
-      <c r="I120" s="28"/>
-      <c r="J120" s="28"/>
+      <c r="B120" s="29"/>
+      <c r="C120" s="29"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="29"/>
+      <c r="F120" s="29"/>
+      <c r="G120" s="29"/>
+      <c r="H120" s="29"/>
+      <c r="I120" s="29"/>
+      <c r="J120" s="29"/>
     </row>
     <row r="121" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="28"/>
-      <c r="C121" s="28"/>
-      <c r="D121" s="28"/>
-      <c r="E121" s="28"/>
-      <c r="F121" s="28"/>
-      <c r="G121" s="28"/>
-      <c r="H121" s="28"/>
-      <c r="I121" s="28"/>
-      <c r="J121" s="28"/>
+      <c r="B121" s="29"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
+      <c r="G121" s="29"/>
+      <c r="H121" s="29"/>
+      <c r="I121" s="29"/>
+      <c r="J121" s="29"/>
     </row>
     <row r="122" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="28"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="28"/>
-      <c r="E122" s="28"/>
-      <c r="F122" s="28"/>
-      <c r="G122" s="28"/>
-      <c r="H122" s="28"/>
-      <c r="I122" s="28"/>
-      <c r="J122" s="28"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="29"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="29"/>
+      <c r="G122" s="29"/>
+      <c r="H122" s="29"/>
+      <c r="I122" s="29"/>
+      <c r="J122" s="29"/>
     </row>
     <row r="123" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="28"/>
-      <c r="C123" s="28"/>
-      <c r="D123" s="28"/>
-      <c r="E123" s="28"/>
-      <c r="F123" s="28"/>
-      <c r="G123" s="28"/>
-      <c r="H123" s="28"/>
-      <c r="I123" s="28"/>
-      <c r="J123" s="28"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="29"/>
     </row>
     <row r="124" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="28"/>
-      <c r="C124" s="28"/>
-      <c r="D124" s="28"/>
-      <c r="E124" s="28"/>
-      <c r="F124" s="28"/>
-      <c r="G124" s="28"/>
-      <c r="H124" s="28"/>
-      <c r="I124" s="28"/>
-      <c r="J124" s="28"/>
+      <c r="B124" s="29"/>
+      <c r="C124" s="29"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="29"/>
+      <c r="F124" s="29"/>
+      <c r="G124" s="29"/>
+      <c r="H124" s="29"/>
+      <c r="I124" s="29"/>
+      <c r="J124" s="29"/>
     </row>
     <row r="125" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="28"/>
-      <c r="C125" s="28"/>
-      <c r="D125" s="28"/>
-      <c r="E125" s="28"/>
-      <c r="F125" s="28"/>
-      <c r="G125" s="28"/>
-      <c r="H125" s="28"/>
-      <c r="I125" s="28"/>
-      <c r="J125" s="28"/>
+      <c r="B125" s="29"/>
+      <c r="C125" s="29"/>
+      <c r="D125" s="29"/>
+      <c r="E125" s="29"/>
+      <c r="F125" s="29"/>
+      <c r="G125" s="29"/>
+      <c r="H125" s="29"/>
+      <c r="I125" s="29"/>
+      <c r="J125" s="29"/>
     </row>
     <row r="126" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="28"/>
-      <c r="C126" s="28"/>
-      <c r="D126" s="28"/>
-      <c r="E126" s="28"/>
-      <c r="F126" s="28"/>
-      <c r="G126" s="28"/>
-      <c r="H126" s="28"/>
-      <c r="I126" s="28"/>
-      <c r="J126" s="28"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="29"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="29"/>
+      <c r="G126" s="29"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="29"/>
+      <c r="J126" s="29"/>
     </row>
     <row r="127" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="28"/>
-      <c r="C127" s="28"/>
-      <c r="D127" s="28"/>
-      <c r="E127" s="28"/>
-      <c r="F127" s="28"/>
-      <c r="G127" s="28"/>
-      <c r="H127" s="28"/>
-      <c r="I127" s="28"/>
-      <c r="J127" s="28"/>
+      <c r="B127" s="29"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
+      <c r="G127" s="29"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
+      <c r="J127" s="29"/>
     </row>
     <row r="128" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="28"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="28"/>
-      <c r="E128" s="28"/>
-      <c r="F128" s="28"/>
-      <c r="G128" s="28"/>
-      <c r="H128" s="28"/>
-      <c r="I128" s="28"/>
-      <c r="J128" s="28"/>
+      <c r="B128" s="29"/>
+      <c r="C128" s="29"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="29"/>
+      <c r="F128" s="29"/>
+      <c r="G128" s="29"/>
+      <c r="H128" s="29"/>
+      <c r="I128" s="29"/>
+      <c r="J128" s="29"/>
     </row>
     <row r="129" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="28"/>
-      <c r="C129" s="28"/>
-      <c r="D129" s="28"/>
-      <c r="E129" s="28"/>
-      <c r="F129" s="28"/>
-      <c r="G129" s="28"/>
-      <c r="H129" s="28"/>
-      <c r="I129" s="28"/>
-      <c r="J129" s="28"/>
+      <c r="B129" s="29"/>
+      <c r="C129" s="29"/>
+      <c r="D129" s="29"/>
+      <c r="E129" s="29"/>
+      <c r="F129" s="29"/>
+      <c r="G129" s="29"/>
+      <c r="H129" s="29"/>
+      <c r="I129" s="29"/>
+      <c r="J129" s="29"/>
     </row>
     <row r="130" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="28"/>
-      <c r="C130" s="28"/>
-      <c r="D130" s="28"/>
-      <c r="E130" s="28"/>
-      <c r="F130" s="28"/>
-      <c r="G130" s="28"/>
-      <c r="H130" s="28"/>
-      <c r="I130" s="28"/>
-      <c r="J130" s="28"/>
+      <c r="B130" s="29"/>
+      <c r="C130" s="29"/>
+      <c r="D130" s="29"/>
+      <c r="E130" s="29"/>
+      <c r="F130" s="29"/>
+      <c r="G130" s="29"/>
+      <c r="H130" s="29"/>
+      <c r="I130" s="29"/>
+      <c r="J130" s="29"/>
     </row>
     <row r="131" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="28"/>
-      <c r="C131" s="28"/>
-      <c r="D131" s="28"/>
-      <c r="E131" s="28"/>
-      <c r="F131" s="28"/>
-      <c r="G131" s="28"/>
-      <c r="H131" s="28"/>
-      <c r="I131" s="28"/>
-      <c r="J131" s="28"/>
+      <c r="B131" s="29"/>
+      <c r="C131" s="29"/>
+      <c r="D131" s="29"/>
+      <c r="E131" s="29"/>
+      <c r="F131" s="29"/>
+      <c r="G131" s="29"/>
+      <c r="H131" s="29"/>
+      <c r="I131" s="29"/>
+      <c r="J131" s="29"/>
     </row>
     <row r="132" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="27" t="s">
+      <c r="B133" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C133" s="28"/>
-      <c r="D133" s="28"/>
-      <c r="E133" s="28"/>
-      <c r="F133" s="28"/>
-      <c r="G133" s="28"/>
-      <c r="H133" s="28"/>
-      <c r="I133" s="28"/>
-      <c r="J133" s="28"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="29"/>
+      <c r="E133" s="29"/>
+      <c r="F133" s="29"/>
+      <c r="G133" s="29"/>
+      <c r="H133" s="29"/>
+      <c r="I133" s="29"/>
+      <c r="J133" s="29"/>
     </row>
     <row r="134" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="28"/>
-      <c r="C134" s="28"/>
-      <c r="D134" s="28"/>
-      <c r="E134" s="28"/>
-      <c r="F134" s="28"/>
-      <c r="G134" s="28"/>
-      <c r="H134" s="28"/>
-      <c r="I134" s="28"/>
-      <c r="J134" s="28"/>
+      <c r="B134" s="29"/>
+      <c r="C134" s="29"/>
+      <c r="D134" s="29"/>
+      <c r="E134" s="29"/>
+      <c r="F134" s="29"/>
+      <c r="G134" s="29"/>
+      <c r="H134" s="29"/>
+      <c r="I134" s="29"/>
+      <c r="J134" s="29"/>
     </row>
     <row r="135" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="28"/>
-      <c r="C135" s="28"/>
-      <c r="D135" s="28"/>
-      <c r="E135" s="28"/>
-      <c r="F135" s="28"/>
-      <c r="G135" s="28"/>
-      <c r="H135" s="28"/>
-      <c r="I135" s="28"/>
-      <c r="J135" s="28"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
+      <c r="D135" s="29"/>
+      <c r="E135" s="29"/>
+      <c r="F135" s="29"/>
+      <c r="G135" s="29"/>
+      <c r="H135" s="29"/>
+      <c r="I135" s="29"/>
+      <c r="J135" s="29"/>
     </row>
     <row r="136" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="28"/>
-      <c r="C136" s="28"/>
-      <c r="D136" s="28"/>
-      <c r="E136" s="28"/>
-      <c r="F136" s="28"/>
-      <c r="G136" s="28"/>
-      <c r="H136" s="28"/>
-      <c r="I136" s="28"/>
-      <c r="J136" s="28"/>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="29"/>
+      <c r="E136" s="29"/>
+      <c r="F136" s="29"/>
+      <c r="G136" s="29"/>
+      <c r="H136" s="29"/>
+      <c r="I136" s="29"/>
+      <c r="J136" s="29"/>
     </row>
     <row r="137" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="28"/>
-      <c r="C137" s="28"/>
-      <c r="D137" s="28"/>
-      <c r="E137" s="28"/>
-      <c r="F137" s="28"/>
-      <c r="G137" s="28"/>
-      <c r="H137" s="28"/>
-      <c r="I137" s="28"/>
-      <c r="J137" s="28"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="29"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="29"/>
+      <c r="F137" s="29"/>
+      <c r="G137" s="29"/>
+      <c r="H137" s="29"/>
+      <c r="I137" s="29"/>
+      <c r="J137" s="29"/>
     </row>
     <row r="138" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="28"/>
-      <c r="C138" s="28"/>
-      <c r="D138" s="28"/>
-      <c r="E138" s="28"/>
-      <c r="F138" s="28"/>
-      <c r="G138" s="28"/>
-      <c r="H138" s="28"/>
-      <c r="I138" s="28"/>
-      <c r="J138" s="28"/>
+      <c r="B138" s="29"/>
+      <c r="C138" s="29"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="29"/>
+      <c r="F138" s="29"/>
+      <c r="G138" s="29"/>
+      <c r="H138" s="29"/>
+      <c r="I138" s="29"/>
+      <c r="J138" s="29"/>
     </row>
     <row r="139" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="28"/>
-      <c r="C139" s="28"/>
-      <c r="D139" s="28"/>
-      <c r="E139" s="28"/>
-      <c r="F139" s="28"/>
-      <c r="G139" s="28"/>
-      <c r="H139" s="28"/>
-      <c r="I139" s="28"/>
-      <c r="J139" s="28"/>
+      <c r="B139" s="29"/>
+      <c r="C139" s="29"/>
+      <c r="D139" s="29"/>
+      <c r="E139" s="29"/>
+      <c r="F139" s="29"/>
+      <c r="G139" s="29"/>
+      <c r="H139" s="29"/>
+      <c r="I139" s="29"/>
+      <c r="J139" s="29"/>
     </row>
     <row r="140" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="28"/>
-      <c r="C140" s="28"/>
-      <c r="D140" s="28"/>
-      <c r="E140" s="28"/>
-      <c r="F140" s="28"/>
-      <c r="G140" s="28"/>
-      <c r="H140" s="28"/>
-      <c r="I140" s="28"/>
-      <c r="J140" s="28"/>
+      <c r="B140" s="29"/>
+      <c r="C140" s="29"/>
+      <c r="D140" s="29"/>
+      <c r="E140" s="29"/>
+      <c r="F140" s="29"/>
+      <c r="G140" s="29"/>
+      <c r="H140" s="29"/>
+      <c r="I140" s="29"/>
+      <c r="J140" s="29"/>
     </row>
     <row r="141" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="28"/>
-      <c r="C141" s="28"/>
-      <c r="D141" s="28"/>
-      <c r="E141" s="28"/>
-      <c r="F141" s="28"/>
-      <c r="G141" s="28"/>
-      <c r="H141" s="28"/>
-      <c r="I141" s="28"/>
-      <c r="J141" s="28"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="29"/>
+      <c r="D141" s="29"/>
+      <c r="E141" s="29"/>
+      <c r="F141" s="29"/>
+      <c r="G141" s="29"/>
+      <c r="H141" s="29"/>
+      <c r="I141" s="29"/>
+      <c r="J141" s="29"/>
     </row>
     <row r="142" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="28"/>
-      <c r="C142" s="28"/>
-      <c r="D142" s="28"/>
-      <c r="E142" s="28"/>
-      <c r="F142" s="28"/>
-      <c r="G142" s="28"/>
-      <c r="H142" s="28"/>
-      <c r="I142" s="28"/>
-      <c r="J142" s="28"/>
+      <c r="B142" s="29"/>
+      <c r="C142" s="29"/>
+      <c r="D142" s="29"/>
+      <c r="E142" s="29"/>
+      <c r="F142" s="29"/>
+      <c r="G142" s="29"/>
+      <c r="H142" s="29"/>
+      <c r="I142" s="29"/>
+      <c r="J142" s="29"/>
     </row>
     <row r="143" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="28"/>
-      <c r="C143" s="28"/>
-      <c r="D143" s="28"/>
-      <c r="E143" s="28"/>
-      <c r="F143" s="28"/>
-      <c r="G143" s="28"/>
-      <c r="H143" s="28"/>
-      <c r="I143" s="28"/>
-      <c r="J143" s="28"/>
+      <c r="B143" s="29"/>
+      <c r="C143" s="29"/>
+      <c r="D143" s="29"/>
+      <c r="E143" s="29"/>
+      <c r="F143" s="29"/>
+      <c r="G143" s="29"/>
+      <c r="H143" s="29"/>
+      <c r="I143" s="29"/>
+      <c r="J143" s="29"/>
     </row>
     <row r="144" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="29" t="s">
+      <c r="B145" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C145" s="28"/>
-      <c r="D145" s="28"/>
-      <c r="E145" s="28"/>
-      <c r="F145" s="28"/>
-      <c r="G145" s="28"/>
-      <c r="H145" s="28"/>
-      <c r="I145" s="28"/>
-      <c r="J145" s="28"/>
+      <c r="C145" s="29"/>
+      <c r="D145" s="29"/>
+      <c r="E145" s="29"/>
+      <c r="F145" s="29"/>
+      <c r="G145" s="29"/>
+      <c r="H145" s="29"/>
+      <c r="I145" s="29"/>
+      <c r="J145" s="29"/>
     </row>
     <row r="146" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="28"/>
-      <c r="C146" s="28"/>
-      <c r="D146" s="28"/>
-      <c r="E146" s="28"/>
-      <c r="F146" s="28"/>
-      <c r="G146" s="28"/>
-      <c r="H146" s="28"/>
-      <c r="I146" s="28"/>
-      <c r="J146" s="28"/>
+      <c r="B146" s="29"/>
+      <c r="C146" s="29"/>
+      <c r="D146" s="29"/>
+      <c r="E146" s="29"/>
+      <c r="F146" s="29"/>
+      <c r="G146" s="29"/>
+      <c r="H146" s="29"/>
+      <c r="I146" s="29"/>
+      <c r="J146" s="29"/>
     </row>
     <row r="147" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="28"/>
-      <c r="C147" s="28"/>
-      <c r="D147" s="28"/>
-      <c r="E147" s="28"/>
-      <c r="F147" s="28"/>
-      <c r="G147" s="28"/>
-      <c r="H147" s="28"/>
-      <c r="I147" s="28"/>
-      <c r="J147" s="28"/>
+      <c r="B147" s="29"/>
+      <c r="C147" s="29"/>
+      <c r="D147" s="29"/>
+      <c r="E147" s="29"/>
+      <c r="F147" s="29"/>
+      <c r="G147" s="29"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
+      <c r="J147" s="29"/>
     </row>
     <row r="148" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="28"/>
-      <c r="C148" s="28"/>
-      <c r="D148" s="28"/>
-      <c r="E148" s="28"/>
-      <c r="F148" s="28"/>
-      <c r="G148" s="28"/>
-      <c r="H148" s="28"/>
-      <c r="I148" s="28"/>
-      <c r="J148" s="28"/>
+      <c r="B148" s="29"/>
+      <c r="C148" s="29"/>
+      <c r="D148" s="29"/>
+      <c r="E148" s="29"/>
+      <c r="F148" s="29"/>
+      <c r="G148" s="29"/>
+      <c r="H148" s="29"/>
+      <c r="I148" s="29"/>
+      <c r="J148" s="29"/>
     </row>
     <row r="149" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="28"/>
-      <c r="C149" s="28"/>
-      <c r="D149" s="28"/>
-      <c r="E149" s="28"/>
-      <c r="F149" s="28"/>
-      <c r="G149" s="28"/>
-      <c r="H149" s="28"/>
-      <c r="I149" s="28"/>
-      <c r="J149" s="28"/>
+      <c r="B149" s="29"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="29"/>
+      <c r="E149" s="29"/>
+      <c r="F149" s="29"/>
+      <c r="G149" s="29"/>
+      <c r="H149" s="29"/>
+      <c r="I149" s="29"/>
+      <c r="J149" s="29"/>
     </row>
     <row r="150" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D150" s="21" t="s">
@@ -6647,8 +6647,8 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6724,7 +6724,9 @@
       <c r="A6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="C6" s="13" t="s">
         <v>52</v>
       </c>
@@ -7809,8 +7811,8 @@
   </sheetPr>
   <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8535,7 +8537,7 @@
       <c r="E32" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F32" s="27" t="s">
         <v>805</v>
       </c>
       <c r="H32" t="s">

</xml_diff>

<commit_message>
update ec terms, added orcid id and voc4cat ids
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="967">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -2626,75 +2626,117 @@
 https://w3id.org/nfdi4cat/voc4cat_0000083</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007201</t>
+  </si>
+  <si>
     <t xml:space="preserve">electrode</t>
   </si>
   <si>
     <t xml:space="preserve">A conductor employed either to determine an electrode potential (at zero current, i.e., for potentiometric experiments), or to determine current during a dynamic electroanalytical measurement. The electronic conductivity of most electrodes is metallic. </t>
   </si>
   <si>
+    <t xml:space="preserve">0009-0008-1278-8890 Michael Götte created the resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007202</t>
+  </si>
+  <si>
     <t xml:space="preserve">working electrode</t>
   </si>
   <si>
     <t xml:space="preserve">The principal electrode during dynamic analyses. The potential of the WE is measured with respect to a reference electrode, while the current passing through the WE is measured with respect to the counter electrode.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007203</t>
+  </si>
+  <si>
     <t xml:space="preserve">counter electrode</t>
   </si>
   <si>
     <t xml:space="preserve">The third electrode in voltammetry and polarography, where the current is measured between the counter and working electrodes. It is rare to monitor the potential of the counter electrode.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007204</t>
+  </si>
+  <si>
     <t xml:space="preserve">reference electrode</t>
   </si>
   <si>
     <t xml:space="preserve">A constant-potential device (e.g., an SHE or SCE) used as a half cell of known potential.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007205</t>
+  </si>
+  <si>
     <t xml:space="preserve">potentiostat</t>
   </si>
   <si>
     <t xml:space="preserve">The instrument employed in dynamic electrochemistry such as voltammetry, allowing three electrodes to be used.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007206</t>
+  </si>
+  <si>
     <t xml:space="preserve">potentiometry</t>
   </si>
   <si>
     <t xml:space="preserve">The techniques and methodology of determining an activity as a function of potential (at zero current). Activity and concentration can often be interchanged at low ionic strength.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007207</t>
+  </si>
+  <si>
     <t xml:space="preserve">chronoamperometry</t>
   </si>
   <si>
     <t xml:space="preserve">The techniques and methodology of studying current as a function of time.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007208</t>
+  </si>
+  <si>
     <t xml:space="preserve">chronopotentiometry</t>
   </si>
   <si>
     <t xml:space="preserve">The techniques and methodology of studying electric potential as a function of time.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007209</t>
+  </si>
+  <si>
     <t xml:space="preserve">electrochemical impedance spectroscopy</t>
   </si>
   <si>
     <t xml:space="preserve">Electrochemical impedance spectroscopy determines the impedance, i.e. the alternating current resistance, of electrochemical systems as a function of the frequency of an alternating voltage or alternating current.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007210</t>
+  </si>
+  <si>
     <t xml:space="preserve">open circuit voltage measurement</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007211</t>
+  </si>
+  <si>
     <t xml:space="preserve">linear sweep voltammetry</t>
   </si>
   <si>
     <t xml:space="preserve">A voltammetry where the voltage changes linearly over time from a initial potential to a final potential.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007212</t>
+  </si>
+  <si>
     <t xml:space="preserve">chronocoulometry</t>
   </si>
   <si>
     <t xml:space="preserve">The techniques and methodology of studying charge as a function of time.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007213</t>
+  </si>
+  <si>
     <t xml:space="preserve">scan rate potential</t>
   </si>
   <si>
@@ -2704,160 +2746,262 @@
     <t xml:space="preserve">sweep rate potential</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007214</t>
+  </si>
+  <si>
     <t xml:space="preserve">lower limit potential</t>
   </si>
   <si>
     <t xml:space="preserve">The minimal potential in a cyclic voltammetry. This is where the sweep turns.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007215</t>
+  </si>
+  <si>
     <t xml:space="preserve">upper limit potential</t>
   </si>
   <si>
     <t xml:space="preserve">The maximal potential in a cyclic voltammetry. This is where the sweep turns.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007216</t>
+  </si>
+  <si>
     <t xml:space="preserve">initial potential</t>
   </si>
   <si>
     <t xml:space="preserve">The potential at which a linear sweep or cyclic voltammetry starts.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007217</t>
+  </si>
+  <si>
     <t xml:space="preserve">final potential</t>
   </si>
   <si>
     <t xml:space="preserve">The potential at which a linear sweep or cyclic voltammetry ends.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007218</t>
+  </si>
+  <si>
     <t xml:space="preserve">step size potential</t>
   </si>
   <si>
     <t xml:space="preserve">The potential at which the potential in a linear sweep or cyclic voltammetry is altered.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007219</t>
+  </si>
+  <si>
     <t xml:space="preserve">electric potential</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007220</t>
+  </si>
+  <si>
     <t xml:space="preserve">current</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007221</t>
+  </si>
+  <si>
     <t xml:space="preserve">current density</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_000722</t>
+  </si>
+  <si>
     <t xml:space="preserve">resistance</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007223</t>
+  </si>
+  <si>
     <t xml:space="preserve">electrochemical environment</t>
   </si>
   <si>
     <t xml:space="preserve">The final environment in which the elctrochemical reaction happens. Includes possibly purged electrolyte.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007224</t>
+  </si>
+  <si>
     <t xml:space="preserve">electrolyte</t>
   </si>
   <si>
     <t xml:space="preserve">An ionic salt to be dissolved in a solvent, or the solution formed by dissolving an ionic salt in a solvent.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007225</t>
+  </si>
+  <si>
     <t xml:space="preserve">purging</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007226</t>
+  </si>
+  <si>
     <t xml:space="preserve">purging gas</t>
   </si>
   <si>
     <t xml:space="preserve">Gas which is used in purging.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007227</t>
+  </si>
+  <si>
     <t xml:space="preserve">purging temperature</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature for which a gas is purged through the reaction chamber.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007228</t>
+  </si>
+  <si>
     <t xml:space="preserve">number of cycles</t>
   </si>
   <si>
     <t xml:space="preserve">The number of cycles in a measurment, such as an cyclic voltammetry.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007229</t>
+  </si>
+  <si>
     <t xml:space="preserve">faradaic efficiency</t>
   </si>
   <si>
     <t xml:space="preserve">The quotient of faradaic current to total current passed.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007230</t>
+  </si>
+  <si>
     <t xml:space="preserve">electrochemical setup</t>
   </si>
   <si>
     <t xml:space="preserve">The collection of instruments and devices used in an electochemical reaction. Can include electrodes, flow cells, beaker, does not include the electrochemical environment.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007231</t>
+  </si>
+  <si>
     <t xml:space="preserve">beaker</t>
   </si>
   <si>
     <t xml:space="preserve">In laboratory equipment, a beaker (also becker or beker) is generally a cylindrical container with a flat bottom.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007232</t>
+  </si>
+  <si>
     <t xml:space="preserve">flow cell</t>
   </si>
   <si>
     <t xml:space="preserve">Electrochemical cell in which analyte solution flows at a constant velocity V through stationary tubular electrode(s).</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007233</t>
+  </si>
+  <si>
     <t xml:space="preserve">rotated ring disk electrode</t>
   </si>
   <si>
     <t xml:space="preserve">Disc electrode within a concentric ring electrode.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007234</t>
+  </si>
+  <si>
     <t xml:space="preserve">total charge transfer</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007235</t>
+  </si>
+  <si>
     <t xml:space="preserve">membrane</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007236</t>
+  </si>
+  <si>
     <t xml:space="preserve">h cell</t>
   </si>
   <si>
     <t xml:space="preserve">The H-Cell is a two-compartment electrochemical cell used for membrane testing, H2 permeation, or any other experiment where two separate electrode chambers are required.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007237</t>
+  </si>
+  <si>
     <t xml:space="preserve">voltammetry</t>
   </si>
   <si>
     <t xml:space="preserve">The techniques and methodology of measuring current as a function of applied potential.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007238</t>
+  </si>
+  <si>
     <t xml:space="preserve">voltammogramm</t>
   </si>
   <si>
     <t xml:space="preserve">A trace of current (as “y“) against applied potential (as “x“).</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007239</t>
+  </si>
+  <si>
     <t xml:space="preserve">angular frequency</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007240</t>
+  </si>
+  <si>
     <t xml:space="preserve">impedance</t>
   </si>
   <si>
     <t xml:space="preserve">AC resistance.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007241</t>
+  </si>
+  <si>
     <t xml:space="preserve">initial angular frequency</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007242</t>
+  </si>
+  <si>
     <t xml:space="preserve">final angular frequency</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007243</t>
+  </si>
+  <si>
     <t xml:space="preserve">rhe compensation</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007244</t>
+  </si>
+  <si>
     <t xml:space="preserve">concentration of a chemical in an electrolyte</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007245</t>
+  </si>
+  <si>
     <t xml:space="preserve">mass coverage</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007246</t>
+  </si>
+  <si>
     <t xml:space="preserve">solvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007247</t>
   </si>
   <si>
     <t xml:space="preserve">solute</t>
@@ -3858,7 +4002,7 @@
   <dimension ref="A11:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="H193:H238 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4041,7 +4185,7 @@
   <dimension ref="A1:J1152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H193:H238 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6760,7 +6904,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="H193:H238 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7928,8 +8072,8 @@
   </sheetPr>
   <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H193" activeCellId="0" sqref="H193:H238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12150,475 +12294,757 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>760</v>
+      </c>
       <c r="B192" s="0" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C192" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D192" s="28" t="s">
-        <v>761</v>
+        <v>762</v>
+      </c>
+      <c r="H192" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>764</v>
+      </c>
       <c r="B193" s="0" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="C193" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D193" s="28" t="s">
+        <v>766</v>
+      </c>
+      <c r="H193" s="0" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>767</v>
+      </c>
       <c r="B194" s="0" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="C194" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D194" s="28" t="s">
-        <v>765</v>
+        <v>769</v>
+      </c>
+      <c r="H194" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>770</v>
+      </c>
       <c r="B195" s="0" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="C195" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D195" s="28" t="s">
-        <v>767</v>
+        <v>772</v>
+      </c>
+      <c r="H195" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>773</v>
+      </c>
       <c r="B196" s="0" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="C196" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D196" s="28" t="s">
-        <v>769</v>
+        <v>775</v>
+      </c>
+      <c r="H196" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>776</v>
+      </c>
       <c r="B197" s="0" t="s">
-        <v>770</v>
+        <v>777</v>
       </c>
       <c r="C197" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D197" s="28" t="s">
-        <v>771</v>
+        <v>778</v>
+      </c>
+      <c r="H197" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>779</v>
+      </c>
       <c r="B198" s="0" t="s">
-        <v>772</v>
+        <v>780</v>
       </c>
       <c r="C198" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D198" s="28" t="s">
-        <v>773</v>
+        <v>781</v>
+      </c>
+      <c r="H198" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>782</v>
+      </c>
       <c r="B199" s="0" t="s">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="C199" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D199" s="28" t="s">
-        <v>775</v>
+        <v>784</v>
+      </c>
+      <c r="H199" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>785</v>
+      </c>
       <c r="B200" s="0" t="s">
-        <v>776</v>
+        <v>786</v>
       </c>
       <c r="C200" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D200" s="28" t="s">
-        <v>777</v>
+        <v>787</v>
+      </c>
+      <c r="H200" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>788</v>
+      </c>
       <c r="B201" s="0" t="s">
-        <v>778</v>
+        <v>789</v>
       </c>
       <c r="C201" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H201" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>790</v>
+      </c>
       <c r="B202" s="0" t="s">
-        <v>779</v>
+        <v>791</v>
       </c>
       <c r="C202" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>780</v>
+        <v>792</v>
+      </c>
+      <c r="H202" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>793</v>
+      </c>
       <c r="B203" s="0" t="s">
-        <v>781</v>
+        <v>794</v>
       </c>
       <c r="C203" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D203" s="28" t="s">
-        <v>782</v>
+        <v>795</v>
+      </c>
+      <c r="H203" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>796</v>
+      </c>
       <c r="B204" s="0" t="s">
-        <v>783</v>
+        <v>797</v>
       </c>
       <c r="C204" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>784</v>
+        <v>798</v>
       </c>
       <c r="F204" s="0" t="s">
-        <v>785</v>
+        <v>799</v>
+      </c>
+      <c r="H204" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>800</v>
+      </c>
       <c r="B205" s="0" t="s">
-        <v>786</v>
+        <v>801</v>
       </c>
       <c r="C205" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>787</v>
+        <v>802</v>
+      </c>
+      <c r="H205" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>803</v>
+      </c>
       <c r="B206" s="0" t="s">
-        <v>788</v>
+        <v>804</v>
       </c>
       <c r="C206" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>789</v>
+        <v>805</v>
+      </c>
+      <c r="H206" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>806</v>
+      </c>
       <c r="B207" s="0" t="s">
-        <v>790</v>
+        <v>807</v>
       </c>
       <c r="C207" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>791</v>
+        <v>808</v>
+      </c>
+      <c r="H207" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>809</v>
+      </c>
       <c r="B208" s="0" t="s">
-        <v>792</v>
+        <v>810</v>
       </c>
       <c r="C208" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>793</v>
+        <v>811</v>
+      </c>
+      <c r="H208" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>812</v>
+      </c>
       <c r="B209" s="0" t="s">
-        <v>794</v>
+        <v>813</v>
       </c>
       <c r="C209" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>795</v>
+        <v>814</v>
+      </c>
+      <c r="H209" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>815</v>
+      </c>
       <c r="B210" s="0" t="s">
-        <v>796</v>
+        <v>816</v>
       </c>
       <c r="C210" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H210" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>817</v>
+      </c>
       <c r="B211" s="0" t="s">
-        <v>797</v>
+        <v>818</v>
       </c>
       <c r="C211" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H211" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>819</v>
+      </c>
       <c r="B212" s="0" t="s">
-        <v>798</v>
+        <v>820</v>
       </c>
       <c r="C212" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H212" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>821</v>
+      </c>
       <c r="B213" s="0" t="s">
-        <v>799</v>
+        <v>822</v>
       </c>
       <c r="C213" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H213" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>823</v>
+      </c>
       <c r="B214" s="0" t="s">
-        <v>800</v>
+        <v>824</v>
       </c>
       <c r="C214" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>801</v>
+        <v>825</v>
+      </c>
+      <c r="H214" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>826</v>
+      </c>
       <c r="B215" s="0" t="s">
-        <v>802</v>
+        <v>827</v>
       </c>
       <c r="C215" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D215" s="28" t="s">
-        <v>803</v>
+        <v>828</v>
+      </c>
+      <c r="H215" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>829</v>
+      </c>
       <c r="B216" s="0" t="s">
-        <v>804</v>
+        <v>830</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H216" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>831</v>
+      </c>
       <c r="B217" s="0" t="s">
-        <v>805</v>
+        <v>832</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>806</v>
+        <v>833</v>
+      </c>
+      <c r="H217" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>834</v>
+      </c>
       <c r="B218" s="0" t="s">
-        <v>807</v>
+        <v>835</v>
       </c>
       <c r="C218" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>808</v>
+        <v>836</v>
+      </c>
+      <c r="H218" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>837</v>
+      </c>
       <c r="B219" s="0" t="s">
-        <v>809</v>
+        <v>838</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>810</v>
+        <v>839</v>
+      </c>
+      <c r="H219" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>840</v>
+      </c>
       <c r="B220" s="0" t="s">
-        <v>811</v>
+        <v>841</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D220" s="28" t="s">
-        <v>812</v>
+        <v>842</v>
+      </c>
+      <c r="H220" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>843</v>
+      </c>
       <c r="B221" s="0" t="s">
-        <v>813</v>
+        <v>844</v>
       </c>
       <c r="C221" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>814</v>
+        <v>845</v>
+      </c>
+      <c r="H221" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>846</v>
+      </c>
       <c r="B222" s="0" t="s">
-        <v>815</v>
+        <v>847</v>
       </c>
       <c r="C222" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>816</v>
+        <v>848</v>
+      </c>
+      <c r="H222" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>849</v>
+      </c>
       <c r="B223" s="0" t="s">
-        <v>817</v>
+        <v>850</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D223" s="28" t="s">
-        <v>818</v>
+        <v>851</v>
+      </c>
+      <c r="H223" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>852</v>
+      </c>
       <c r="B224" s="0" t="s">
-        <v>819</v>
+        <v>853</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D224" s="28" t="s">
-        <v>820</v>
+        <v>854</v>
+      </c>
+      <c r="H224" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>855</v>
+      </c>
       <c r="B225" s="0" t="s">
-        <v>821</v>
+        <v>856</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H225" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>857</v>
+      </c>
       <c r="B226" s="0" t="s">
-        <v>822</v>
+        <v>858</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H226" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>859</v>
+      </c>
       <c r="B227" s="0" t="s">
-        <v>823</v>
+        <v>860</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D227" s="28" t="s">
-        <v>824</v>
+        <v>861</v>
+      </c>
+      <c r="H227" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>862</v>
+      </c>
       <c r="B228" s="0" t="s">
-        <v>825</v>
+        <v>863</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D228" s="28" t="s">
-        <v>826</v>
+        <v>864</v>
+      </c>
+      <c r="H228" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>865</v>
+      </c>
       <c r="B229" s="0" t="s">
-        <v>827</v>
+        <v>866</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D229" s="28" t="s">
-        <v>828</v>
+        <v>867</v>
+      </c>
+      <c r="H229" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>868</v>
+      </c>
       <c r="B230" s="0" t="s">
-        <v>829</v>
+        <v>869</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H230" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>870</v>
+      </c>
       <c r="B231" s="0" t="s">
-        <v>830</v>
+        <v>871</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D231" s="28" t="s">
-        <v>831</v>
+        <v>872</v>
+      </c>
+      <c r="H231" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>873</v>
+      </c>
       <c r="B232" s="0" t="s">
-        <v>832</v>
+        <v>874</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H232" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>875</v>
+      </c>
       <c r="B233" s="0" t="s">
-        <v>833</v>
+        <v>876</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H233" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>877</v>
+      </c>
       <c r="B234" s="0" t="s">
-        <v>834</v>
+        <v>878</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H234" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>879</v>
+      </c>
       <c r="B235" s="0" t="s">
-        <v>835</v>
+        <v>880</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H235" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>881</v>
+      </c>
       <c r="B236" s="0" t="s">
-        <v>836</v>
+        <v>882</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H236" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>883</v>
+      </c>
       <c r="B237" s="0" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="H237" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>885</v>
+      </c>
       <c r="B238" s="0" t="s">
-        <v>838</v>
+        <v>886</v>
       </c>
       <c r="C238" s="0" t="s">
         <v>84</v>
+      </c>
+      <c r="H238" s="0" t="s">
+        <v>763</v>
       </c>
     </row>
   </sheetData>
@@ -12647,7 +13073,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H193:H238 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12658,7 +13084,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>839</v>
+        <v>887</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12666,19 +13092,19 @@
         <v>74</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>840</v>
+        <v>888</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>841</v>
+        <v>889</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>842</v>
+        <v>890</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>843</v>
+        <v>891</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>844</v>
+        <v>892</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13943,7 +14369,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H193:H238 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13957,38 +14383,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>845</v>
+        <v>893</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>846</v>
+        <v>894</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>847</v>
+        <v>895</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>848</v>
+        <v>896</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>849</v>
+        <v>897</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>850</v>
+        <v>898</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>851</v>
+        <v>899</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>852</v>
+        <v>900</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>853</v>
+        <v>901</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>854</v>
+        <v>902</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>120</v>
@@ -13996,16 +14422,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>855</v>
+        <v>903</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>856</v>
+        <v>904</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>857</v>
+        <v>905</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>858</v>
+        <v>906</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>120</v>
@@ -14145,7 +14571,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="H193:H238 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14155,242 +14581,242 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>859</v>
+        <v>907</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>860</v>
+        <v>908</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>861</v>
+        <v>909</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>862</v>
+        <v>910</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>863</v>
+        <v>911</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>864</v>
+        <v>912</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>865</v>
+        <v>913</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>866</v>
+        <v>914</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>867</v>
+        <v>915</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>868</v>
+        <v>916</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>869</v>
+        <v>917</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>870</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>871</v>
+        <v>919</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>872</v>
+        <v>920</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>873</v>
+        <v>921</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>874</v>
+        <v>922</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>875</v>
+        <v>923</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>876</v>
+        <v>924</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>877</v>
+        <v>925</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>878</v>
+        <v>926</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>879</v>
+        <v>927</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>880</v>
+        <v>928</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>881</v>
+        <v>929</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>882</v>
+        <v>930</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>883</v>
+        <v>931</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>884</v>
+        <v>932</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>885</v>
+        <v>933</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>886</v>
+        <v>934</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>887</v>
+        <v>935</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>888</v>
+        <v>936</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>889</v>
+        <v>937</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>890</v>
+        <v>938</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>891</v>
+        <v>939</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>892</v>
+        <v>940</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>893</v>
+        <v>941</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>894</v>
+        <v>942</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>895</v>
+        <v>943</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>896</v>
+        <v>944</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>897</v>
+        <v>945</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>898</v>
+        <v>946</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>899</v>
+        <v>947</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>900</v>
+        <v>948</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>901</v>
+        <v>949</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>902</v>
+        <v>950</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>903</v>
+        <v>951</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>904</v>
+        <v>952</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>905</v>
+        <v>953</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>906</v>
+        <v>954</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>907</v>
+        <v>955</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>908</v>
+        <v>956</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>909</v>
+        <v>957</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>910</v>
+        <v>958</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>911</v>
+        <v>959</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>912</v>
+        <v>960</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>913</v>
+        <v>961</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>914</v>
+        <v>962</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>915</v>
+        <v>963</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>916</v>
+        <v>964</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>917</v>
+        <v>965</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>918</v>
+        <v>966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added galvanic and electrolytic cell
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="1033">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -2722,7 +2722,7 @@
     <t xml:space="preserve">electrochemical impedance spectroscopy </t>
   </si>
   <si>
-    <t xml:space="preserve">Electrochemical impedance spectroscopy is a powerful tool for examining processes occurring at electrode surfaces. A small amplitude ac (sinusoidal) excitation signal (potential or current), covering a wide range of frequencies, is applied to the system under investigation and the response (current or voltage or another signal of interest) is measured. It is routinely used in electrode kinetics and mechanism investigations, and in the characterization of batteries, fuel cells, and corrosion phenomena. Abbreviated as "EIS".  electrochemical irreversibility</t>
+    <t xml:space="preserve">Electrochemical impedance spectroscopy is a powerful tool for examining processes occurring at electrode surfaces. A small amplitude ac (sinusoidal) excitation signal (potential or current), covering a wide range of frequencies, is applied to the system under investigation and the response (current or voltage or another signal of interest) is measured. It is routinely used in electrode kinetics and mechanism investigations, and in the characterization of batteries, fuel cells, and corrosion phenomena.</t>
   </si>
   <si>
     <t xml:space="preserve">EIS</t>
@@ -2818,7 +2818,7 @@
     <t xml:space="preserve">step size potential</t>
   </si>
   <si>
-    <t xml:space="preserve">The potential at which the potential in a linear sweep or cyclic voltammetry is altered.</t>
+    <t xml:space="preserve">The potential difference at which the potential in a linear sweep or cyclic voltammetry is altered.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007219</t>
@@ -3061,7 +3061,7 @@
     <t xml:space="preserve">reversible hydrogen electrode</t>
   </si>
   <si>
-    <t xml:space="preserve">A commonly used reference electrode. A hydrogen electrode immersed directly into the electrolyte of the electrochemical cell and usually (unless otherwise stated) operated with one atmosphere pressure hydrogen gas. The equilibrium potential depends on the hydrogen ion concentration (strictly speaking, activity) of the cell electrolyte. Abbreviated as "RHE".</t>
+    <t xml:space="preserve">A commonly used reference electrode. A hydrogen electrode immersed directly into the electrolyte of the electrochemical cell and usually (unless otherwise stated) operated with one atmosphere pressure hydrogen gas. The equilibrium potential depends on the hydrogen ion concentration (strictly speaking, activity) of the cell electrolyte.</t>
   </si>
   <si>
     <t xml:space="preserve">RHE</t>
@@ -3124,6 +3124,9 @@
     <t xml:space="preserve">A device that converts chemical energy into electrical energy or vice versa when a chemical reaction is occurring in the cell. Typically, it consists of two metal electrodes immersed into an aqueous solution (electrolyte) with electrode reactions occurring at the electrode-solution surfaces. See also galvanic cell and electrolytic cell.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007256, https://w3id.org/nfdi4cat/voc4cat_0007257</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007250</t>
   </si>
   <si>
@@ -3182,6 +3185,24 @@
   </si>
   <si>
     <t xml:space="preserve">The electrode where oxidation occurs in an electrochemical cell. It is the positive electrode in an electrolytic cell, while it is the negative electrode in a galvanic cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">galvanic cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An electrochemical cell that converts chemical energy into electrical energy. A cell in which chemical reactions occur spontaneously at the electrodes when they are connected through an external circuit, producing an electrical current.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electrolytic cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An electrochemical cell that converts electrical energy into chemical energy. The chemical reactions do not occur "spontaneously" at the electrodes when they are connected through an external circuit. The reaction must be forced by applying an external electrical current.</t>
   </si>
   <si>
     <t xml:space="preserve">Concept Relations</t>
@@ -4095,9 +4116,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>579240</xdr:colOff>
+      <xdr:colOff>578880</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4111,8 +4132,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1377360" y="304920"/>
-          <a:ext cx="5922720" cy="1541520"/>
+          <a:off x="1377720" y="304920"/>
+          <a:ext cx="5925960" cy="1541160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4192,7 +4213,7 @@
       <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -4375,7 +4396,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -7094,7 +7115,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -8257,13 +8278,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I246"/>
+  <dimension ref="A1:I248"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G241" activeCellId="0" sqref="G241"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A202" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A240" activeCellId="0" sqref="A240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -13372,25 +13393,28 @@
       <c r="D240" s="28" t="s">
         <v>925</v>
       </c>
+      <c r="G240" s="0" t="s">
+        <v>926</v>
+      </c>
       <c r="H240" s="0" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C241" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D241" s="0" t="s">
-        <v>928</v>
-      </c>
-      <c r="G241" s="30" t="s">
         <v>929</v>
+      </c>
+      <c r="G241" s="29" t="s">
+        <v>930</v>
       </c>
       <c r="H241" s="0" t="s">
         <v>764</v>
@@ -13398,19 +13422,19 @@
     </row>
     <row r="242" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C242" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D242" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="F242" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="H242" s="0" t="s">
         <v>764</v>
@@ -13418,16 +13442,16 @@
     </row>
     <row r="243" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C243" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D243" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="H243" s="0" t="s">
         <v>764</v>
@@ -13435,16 +13459,16 @@
     </row>
     <row r="244" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C244" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="H244" s="0" t="s">
         <v>764</v>
@@ -13452,16 +13476,16 @@
     </row>
     <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D245" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="H245" s="0" t="s">
         <v>764</v>
@@ -13469,37 +13493,74 @@
     </row>
     <row r="246" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C246" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D246" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="H246" s="0" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>947</v>
+      </c>
+      <c r="B247" s="30" t="s">
+        <v>948</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D247" s="28" t="s">
+        <v>949</v>
+      </c>
+      <c r="H247" s="0" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="B248" s="30" t="s">
+        <v>951</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D248" s="28" t="s">
+        <v>952</v>
+      </c>
+      <c r="H248" s="0" t="s">
         <v>764</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId2" display="https://www.w3.org/TR/2010/NOTE-curie-20101216/"/>
-    <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007219"/>
+    <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218, https://w3id.org/nfdi4cat/voc4cat_0007219"/>
     <hyperlink ref="A213" r:id="rId4" display="https://w3id.org/nfdi4cat/voc4cat_0007222"/>
-    <hyperlink ref="G228" r:id="rId5" display="https://w3id.org/nfdi4cat/voc4cat_0000082"/>
-    <hyperlink ref="G230" r:id="rId6" display="https://w3id.org/nfdi4cat/voc4cat_0007242"/>
+    <hyperlink ref="G228" r:id="rId5" display="https://w3id.org/nfdi4cat/voc4cat_0007211, https://w3id.org/nfdi4cat/voc4cat_0000082"/>
+    <hyperlink ref="G230" r:id="rId6" display="https://w3id.org/nfdi4cat/voc4cat_0007241, https://w3id.org/nfdi4cat/voc4cat_0007242"/>
     <hyperlink ref="A239" r:id="rId7" display="https://w3id.org/nfdi4cat/voc4cat_0007248"/>
     <hyperlink ref="A240" r:id="rId8" display="https://w3id.org/nfdi4cat/voc4cat_0007249"/>
-    <hyperlink ref="A241" r:id="rId9" display="https://w3id.org/nfdi4cat/voc4cat_0007250"/>
-    <hyperlink ref="G241" r:id="rId10" display="https://w3id.org/nfdi4cat/voc4cat_0007236"/>
-    <hyperlink ref="A242" r:id="rId11" display="https://w3id.org/nfdi4cat/voc4cat_0007251"/>
-    <hyperlink ref="A243" r:id="rId12" display="https://w3id.org/nfdi4cat/voc4cat_0007252"/>
-    <hyperlink ref="A244" r:id="rId13" display="https://w3id.org/nfdi4cat/voc4cat_0007253"/>
-    <hyperlink ref="A245" r:id="rId14" display="https://w3id.org/nfdi4cat/voc4cat_0007254"/>
-    <hyperlink ref="A246" r:id="rId15" display="https://w3id.org/nfdi4cat/voc4cat_0007255"/>
+    <hyperlink ref="G240" r:id="rId9" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
+    <hyperlink ref="A241" r:id="rId10" display="https://w3id.org/nfdi4cat/voc4cat_0007250"/>
+    <hyperlink ref="G241" r:id="rId11" display="https://w3id.org/nfdi4cat/voc4cat_0007205, https://w3id.org/nfdi4cat/voc4cat_0007231, https://w3id.org/nfdi4cat/voc4cat_0007232, https://w3id.org/nfdi4cat/voc4cat_0007235, https://w3id.org/nfdi4cat/voc4cat_0007248, https://w3id.org/nfdi4cat/voc4cat_0007236"/>
+    <hyperlink ref="A242" r:id="rId12" display="https://w3id.org/nfdi4cat/voc4cat_0007251"/>
+    <hyperlink ref="A243" r:id="rId13" display="https://w3id.org/nfdi4cat/voc4cat_0007252"/>
+    <hyperlink ref="A244" r:id="rId14" display="https://w3id.org/nfdi4cat/voc4cat_0007253"/>
+    <hyperlink ref="A245" r:id="rId15" display="https://w3id.org/nfdi4cat/voc4cat_0007254"/>
+    <hyperlink ref="A246" r:id="rId16" display="https://w3id.org/nfdi4cat/voc4cat_0007255"/>
+    <hyperlink ref="A247" r:id="rId17" display="https://w3id.org/nfdi4cat/voc4cat_0007256"/>
+    <hyperlink ref="A248" r:id="rId18" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -13508,9 +13569,9 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId16"/>
+  <legacyDrawing r:id="rId19"/>
   <tableParts>
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
@@ -13526,7 +13587,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -13534,7 +13595,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>946</v>
+        <v>953</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13542,19 +13603,19 @@
         <v>74</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>947</v>
+        <v>954</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14822,7 +14883,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -14833,38 +14894,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>960</v>
+        <v>967</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>120</v>
@@ -14872,16 +14933,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>962</v>
+        <v>969</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>964</v>
+        <v>971</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>965</v>
+        <v>972</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>120</v>
@@ -15024,249 +15085,249 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>969</v>
+        <v>976</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>976</v>
+        <v>983</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>977</v>
+        <v>984</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>978</v>
+        <v>985</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>979</v>
+        <v>986</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>980</v>
+        <v>987</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>982</v>
+        <v>989</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>983</v>
+        <v>990</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>984</v>
+        <v>991</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>985</v>
+        <v>992</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>986</v>
+        <v>993</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>988</v>
+        <v>995</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>989</v>
+        <v>996</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>990</v>
+        <v>997</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>991</v>
+        <v>998</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>992</v>
+        <v>999</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>994</v>
+        <v>1001</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>996</v>
+        <v>1003</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>997</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>998</v>
+        <v>1005</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>999</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1001</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1003</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1004</v>
+        <v>1011</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>1005</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1008</v>
+        <v>1015</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>1009</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1010</v>
+        <v>1017</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1012</v>
+        <v>1019</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>1013</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1014</v>
+        <v>1021</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1015</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1016</v>
+        <v>1023</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1017</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1018</v>
+        <v>1025</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1019</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1020</v>
+        <v>1027</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>1021</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1022</v>
+        <v>1029</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added active area and faradaic current
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1040">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -2842,6 +2842,9 @@
     <t xml:space="preserve">The movement of electrical charges in a conductor; carried by electrons in an electronic conductor (electronic current) or by ions in an ionic conductor (ionic current). </t>
   </si>
   <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007259</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007221</t>
   </si>
   <si>
@@ -3203,6 +3206,24 @@
   </si>
   <si>
     <t xml:space="preserve">An electrochemical cell that converts electrical energy into chemical energy. The chemical reactions do not occur "spontaneously" at the electrodes when they are connected through an external circuit. The reaction must be forced by applying an external electrical current.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In contrast to substrate area, the actual area of a sample or electrode which is active.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true electrode area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faradaic current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current that is flowing through an electrochemical cell and is causing (or is caused by) chemical reactions (charge transfer) occurring at the electrode surfaces. </t>
   </si>
   <si>
     <t xml:space="preserve">Concept Relations</t>
@@ -3869,7 +3890,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3988,6 +4009,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -4210,7 +4235,7 @@
   <dimension ref="A11:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="211:211 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4393,7 +4418,7 @@
   <dimension ref="A1:J1152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="211:211 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7112,7 +7137,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="211:211 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8278,10 +8303,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I248"/>
+  <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A202" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A240" activeCellId="0" sqref="A240"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A211" activeCellId="0" sqref="211:211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12873,22 +12898,25 @@
       <c r="D211" s="0" t="s">
         <v>831</v>
       </c>
+      <c r="G211" s="0" t="s">
+        <v>832</v>
+      </c>
       <c r="H211" s="0" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C212" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="H212" s="0" t="s">
         <v>764</v>
@@ -12896,16 +12924,16 @@
     </row>
     <row r="213" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C213" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="H213" s="0" t="s">
         <v>764</v>
@@ -12913,16 +12941,16 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C214" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="H214" s="0" t="s">
         <v>764</v>
@@ -12930,16 +12958,16 @@
     </row>
     <row r="215" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C215" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D215" s="28" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="H215" s="0" t="s">
         <v>764</v>
@@ -12947,16 +12975,16 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="H216" s="0" t="s">
         <v>764</v>
@@ -12964,16 +12992,16 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="H217" s="0" t="s">
         <v>764</v>
@@ -12981,16 +13009,16 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C218" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="H218" s="0" t="s">
         <v>764</v>
@@ -12998,16 +13026,16 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="H219" s="0" t="s">
         <v>764</v>
@@ -13015,16 +13043,16 @@
     </row>
     <row r="220" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D220" s="28" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H220" s="0" t="s">
         <v>764</v>
@@ -13032,16 +13060,16 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C221" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H221" s="0" t="s">
         <v>764</v>
@@ -13049,19 +13077,19 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C222" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="F222" s="0" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="G222" s="29"/>
       <c r="H222" s="0" t="s">
@@ -13070,16 +13098,16 @@
     </row>
     <row r="223" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D223" s="28" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="G223" s="29"/>
       <c r="H223" s="0" t="s">
@@ -13088,16 +13116,16 @@
     </row>
     <row r="224" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D224" s="28" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="G224" s="29"/>
       <c r="H224" s="0" t="s">
@@ -13106,16 +13134,16 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="H225" s="0" t="s">
         <v>764</v>
@@ -13123,19 +13151,19 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="F226" s="0" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="G226" s="29"/>
       <c r="H226" s="0" t="s">
@@ -13144,19 +13172,19 @@
     </row>
     <row r="227" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D227" s="28" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="F227" s="0" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="G227" s="29"/>
       <c r="H227" s="0" t="s">
@@ -13165,19 +13193,19 @@
     </row>
     <row r="228" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D228" s="28" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="G228" s="0" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="H228" s="0" t="s">
         <v>764</v>
@@ -13185,16 +13213,16 @@
     </row>
     <row r="229" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D229" s="28" t="s">
-        <v>889</v>
+      <c r="D229" s="30" t="s">
+        <v>890</v>
       </c>
       <c r="H229" s="0" t="s">
         <v>764</v>
@@ -13202,19 +13230,19 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D230" s="0" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="G230" s="0" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H230" s="0" t="s">
         <v>764</v>
@@ -13222,16 +13250,16 @@
     </row>
     <row r="231" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D231" s="28" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="H231" s="0" t="s">
         <v>764</v>
@@ -13239,16 +13267,16 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D232" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="H232" s="0" t="s">
         <v>764</v>
@@ -13256,16 +13284,16 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D233" s="0" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="H233" s="0" t="s">
         <v>764</v>
@@ -13273,19 +13301,19 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D234" s="0" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="F234" s="0" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="H234" s="0" t="s">
         <v>764</v>
@@ -13293,16 +13321,16 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D235" s="0" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="H235" s="0" t="s">
         <v>764</v>
@@ -13310,16 +13338,16 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D236" s="0" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="H236" s="0" t="s">
         <v>764</v>
@@ -13327,16 +13355,16 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D237" s="0" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="H237" s="0" t="s">
         <v>764</v>
@@ -13344,16 +13372,16 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C238" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D238" s="0" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H238" s="0" t="s">
         <v>764</v>
@@ -13361,19 +13389,19 @@
     </row>
     <row r="239" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C239" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D239" s="28" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F239" s="0" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="G239" s="29"/>
       <c r="H239" s="0" t="s">
@@ -13382,19 +13410,19 @@
     </row>
     <row r="240" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C240" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D240" s="28" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="G240" s="0" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="H240" s="0" t="s">
         <v>764</v>
@@ -13402,19 +13430,19 @@
     </row>
     <row r="241" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C241" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D241" s="0" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="G241" s="29" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="H241" s="0" t="s">
         <v>764</v>
@@ -13422,19 +13450,19 @@
     </row>
     <row r="242" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C242" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D242" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="F242" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="H242" s="0" t="s">
         <v>764</v>
@@ -13442,16 +13470,16 @@
     </row>
     <row r="243" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C243" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D243" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="H243" s="0" t="s">
         <v>764</v>
@@ -13459,16 +13487,16 @@
     </row>
     <row r="244" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C244" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="H244" s="0" t="s">
         <v>764</v>
@@ -13476,16 +13504,16 @@
     </row>
     <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D245" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="H245" s="0" t="s">
         <v>764</v>
@@ -13493,16 +13521,16 @@
     </row>
     <row r="246" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C246" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D246" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="H246" s="0" t="s">
         <v>764</v>
@@ -13510,16 +13538,16 @@
     </row>
     <row r="247" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>947</v>
-      </c>
-      <c r="B247" s="30" t="s">
         <v>948</v>
       </c>
+      <c r="B247" s="31" t="s">
+        <v>949</v>
+      </c>
       <c r="C247" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D247" s="28" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="H247" s="0" t="s">
         <v>764</v>
@@ -13527,18 +13555,55 @@
     </row>
     <row r="248" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>950</v>
-      </c>
-      <c r="B248" s="30" t="s">
         <v>951</v>
       </c>
+      <c r="B248" s="31" t="s">
+        <v>952</v>
+      </c>
       <c r="C248" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D248" s="28" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="H248" s="0" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="B249" s="31" t="s">
+        <v>955</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D249" s="28" t="s">
+        <v>956</v>
+      </c>
+      <c r="G249" s="0" t="s">
+        <v>957</v>
+      </c>
+      <c r="H249" s="0" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="B250" s="31" t="s">
+        <v>958</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D250" s="28" t="s">
+        <v>959</v>
+      </c>
+      <c r="H250" s="0" t="s">
         <v>764</v>
       </c>
     </row>
@@ -13546,21 +13611,24 @@
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId2" display="https://www.w3.org/TR/2010/NOTE-curie-20101216/"/>
     <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218, https://w3id.org/nfdi4cat/voc4cat_0007219"/>
-    <hyperlink ref="A213" r:id="rId4" display="https://w3id.org/nfdi4cat/voc4cat_0007222"/>
-    <hyperlink ref="G228" r:id="rId5" display="https://w3id.org/nfdi4cat/voc4cat_0007211, https://w3id.org/nfdi4cat/voc4cat_0000082"/>
-    <hyperlink ref="G230" r:id="rId6" display="https://w3id.org/nfdi4cat/voc4cat_0007241, https://w3id.org/nfdi4cat/voc4cat_0007242"/>
-    <hyperlink ref="A239" r:id="rId7" display="https://w3id.org/nfdi4cat/voc4cat_0007248"/>
-    <hyperlink ref="A240" r:id="rId8" display="https://w3id.org/nfdi4cat/voc4cat_0007249"/>
-    <hyperlink ref="G240" r:id="rId9" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
-    <hyperlink ref="A241" r:id="rId10" display="https://w3id.org/nfdi4cat/voc4cat_0007250"/>
-    <hyperlink ref="G241" r:id="rId11" display="https://w3id.org/nfdi4cat/voc4cat_0007205, https://w3id.org/nfdi4cat/voc4cat_0007231, https://w3id.org/nfdi4cat/voc4cat_0007232, https://w3id.org/nfdi4cat/voc4cat_0007235, https://w3id.org/nfdi4cat/voc4cat_0007248, https://w3id.org/nfdi4cat/voc4cat_0007236"/>
-    <hyperlink ref="A242" r:id="rId12" display="https://w3id.org/nfdi4cat/voc4cat_0007251"/>
-    <hyperlink ref="A243" r:id="rId13" display="https://w3id.org/nfdi4cat/voc4cat_0007252"/>
-    <hyperlink ref="A244" r:id="rId14" display="https://w3id.org/nfdi4cat/voc4cat_0007253"/>
-    <hyperlink ref="A245" r:id="rId15" display="https://w3id.org/nfdi4cat/voc4cat_0007254"/>
-    <hyperlink ref="A246" r:id="rId16" display="https://w3id.org/nfdi4cat/voc4cat_0007255"/>
-    <hyperlink ref="A247" r:id="rId17" display="https://w3id.org/nfdi4cat/voc4cat_0007256"/>
-    <hyperlink ref="A248" r:id="rId18" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
+    <hyperlink ref="G211" r:id="rId4" display="https://w3id.org/nfdi4cat/voc4cat_0007259"/>
+    <hyperlink ref="A213" r:id="rId5" display="https://w3id.org/nfdi4cat/voc4cat_0007222"/>
+    <hyperlink ref="G228" r:id="rId6" display="https://w3id.org/nfdi4cat/voc4cat_0007211, https://w3id.org/nfdi4cat/voc4cat_0000082"/>
+    <hyperlink ref="G230" r:id="rId7" display="https://w3id.org/nfdi4cat/voc4cat_0007241, https://w3id.org/nfdi4cat/voc4cat_0007242"/>
+    <hyperlink ref="A239" r:id="rId8" display="https://w3id.org/nfdi4cat/voc4cat_0007248"/>
+    <hyperlink ref="A240" r:id="rId9" display="https://w3id.org/nfdi4cat/voc4cat_0007249"/>
+    <hyperlink ref="G240" r:id="rId10" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
+    <hyperlink ref="A241" r:id="rId11" display="https://w3id.org/nfdi4cat/voc4cat_0007250"/>
+    <hyperlink ref="G241" r:id="rId12" display="https://w3id.org/nfdi4cat/voc4cat_0007205, https://w3id.org/nfdi4cat/voc4cat_0007231, https://w3id.org/nfdi4cat/voc4cat_0007232, https://w3id.org/nfdi4cat/voc4cat_0007235, https://w3id.org/nfdi4cat/voc4cat_0007248, https://w3id.org/nfdi4cat/voc4cat_0007236"/>
+    <hyperlink ref="A242" r:id="rId13" display="https://w3id.org/nfdi4cat/voc4cat_0007251"/>
+    <hyperlink ref="A243" r:id="rId14" display="https://w3id.org/nfdi4cat/voc4cat_0007252"/>
+    <hyperlink ref="A244" r:id="rId15" display="https://w3id.org/nfdi4cat/voc4cat_0007253"/>
+    <hyperlink ref="A245" r:id="rId16" display="https://w3id.org/nfdi4cat/voc4cat_0007254"/>
+    <hyperlink ref="A246" r:id="rId17" display="https://w3id.org/nfdi4cat/voc4cat_0007255"/>
+    <hyperlink ref="A247" r:id="rId18" display="https://w3id.org/nfdi4cat/voc4cat_0007256"/>
+    <hyperlink ref="A248" r:id="rId19" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
+    <hyperlink ref="A249" r:id="rId20" display="https://w3id.org/nfdi4cat/voc4cat_0007258"/>
+    <hyperlink ref="A250" r:id="rId21" display="https://w3id.org/nfdi4cat/voc4cat_0007259"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -13569,9 +13637,9 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId19"/>
+  <legacyDrawing r:id="rId22"/>
   <tableParts>
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
@@ -13584,7 +13652,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="211:211 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13595,7 +13663,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13603,19 +13671,19 @@
         <v>74</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14880,7 +14948,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="211:211 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14894,38 +14962,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>960</v>
+        <v>967</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>962</v>
+        <v>969</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>964</v>
+        <v>971</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>965</v>
+        <v>972</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>120</v>
@@ -14933,16 +15001,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>969</v>
+        <v>976</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>120</v>
@@ -15082,7 +15150,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="211:211 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15092,242 +15160,242 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>976</v>
+        <v>983</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>977</v>
+        <v>984</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>978</v>
+        <v>985</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>979</v>
+        <v>986</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>980</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>982</v>
+        <v>989</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>983</v>
+        <v>990</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>984</v>
+        <v>991</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>985</v>
+        <v>992</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>986</v>
+        <v>993</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>988</v>
+        <v>995</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>989</v>
+        <v>996</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>990</v>
+        <v>997</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>991</v>
+        <v>998</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>992</v>
+        <v>999</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>994</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>996</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>997</v>
+        <v>1004</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>998</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>999</v>
+        <v>1006</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>1001</v>
+        <v>1008</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1002</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>1003</v>
+        <v>1010</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>1004</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>1005</v>
+        <v>1012</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>1006</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>1007</v>
+        <v>1014</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1008</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>1009</v>
+        <v>1016</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1010</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>1012</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1013</v>
+        <v>1020</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1014</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1015</v>
+        <v>1022</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>1016</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1017</v>
+        <v>1024</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>1018</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1019</v>
+        <v>1026</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>1020</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1021</v>
+        <v>1028</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1022</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1026</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1027</v>
+        <v>1034</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>1028</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1029</v>
+        <v>1036</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1030</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1031</v>
+        <v>1038</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>1032</v>
+        <v>1039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix active area
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -4235,7 +4235,7 @@
   <dimension ref="A11:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="211:211 J12"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="F249 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4418,7 +4418,7 @@
   <dimension ref="A1:J1152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="211:211 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F249 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7137,7 +7137,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="211:211 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="F249 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8305,8 +8305,8 @@
   </sheetPr>
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A211" activeCellId="0" sqref="211:211"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F249" activeCellId="0" sqref="F249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13583,7 +13583,7 @@
       <c r="D249" s="28" t="s">
         <v>956</v>
       </c>
-      <c r="G249" s="0" t="s">
+      <c r="F249" s="0" t="s">
         <v>957</v>
       </c>
       <c r="H249" s="0" t="s">
@@ -13652,7 +13652,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="211:211 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="F249 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14948,7 +14948,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="211:211 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="F249 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15150,7 +15150,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="211:211 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F249 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
resolved most comments from david
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -2722,7 +2722,7 @@
     <t xml:space="preserve">electrochemical impedance spectroscopy </t>
   </si>
   <si>
-    <t xml:space="preserve">Electrochemical impedance spectroscopy is a powerful tool for examining processes occurring at electrode surfaces. A small amplitude ac (sinusoidal) excitation signal (potential or current), covering a wide range of frequencies, is applied to the system under investigation and the response (current or voltage or another signal of interest) is measured. It is routinely used in electrode kinetics and mechanism investigations, and in the characterization of batteries, fuel cells, and corrosion phenomena.</t>
+    <t xml:space="preserve">A powerful tool for examining processes occurring at electrode surfaces. A small amplitude ac (sinusoidal) excitation signal (potential or current), covering a wide range of frequencies, is applied to the system under investigation and the response (current or voltage or another signal of interest) is measured. It is routinely used in electrode kinetics and mechanism investigations, and in the characterization of batteries, fuel cells, and corrosion phenomena.</t>
   </si>
   <si>
     <t xml:space="preserve">EIS</t>
@@ -2830,7 +2830,7 @@
     <t xml:space="preserve">The electrical potential difference between two points in a circuit is the cause of the flow of a current.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218, https://w3id.org/nfdi4cat/voc4cat_0007219</t>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007220</t>
@@ -2953,13 +2953,13 @@
     <t xml:space="preserve">flow cell</t>
   </si>
   <si>
-    <t xml:space="preserve">Electrochemical cell in which analyte solution flows at a constant velocity V through stationary tubular electrode(s).</t>
+    <t xml:space="preserve">Electrochemical cell in which analyte solution flows at a constant velocity through stationary tubular electrode(s).</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007233</t>
   </si>
   <si>
-    <t xml:space="preserve">cycle</t>
+    <t xml:space="preserve">voltammetry cycle</t>
   </si>
   <si>
     <t xml:space="preserve">In voltammetry: a complementary pair of forward and reverse potential sweeps.</t>
@@ -2989,13 +2989,13 @@
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007236</t>
   </si>
   <si>
-    <t xml:space="preserve">h cell</t>
+    <t xml:space="preserve">H cell</t>
   </si>
   <si>
     <t xml:space="preserve">The H-Cell is a two-compartment electrochemical cell used for membrane testing, hydrogen permeation, or any other experiment where two separate electrode chambers are required.</t>
   </si>
   <si>
-    <t xml:space="preserve">H-cell, H-cell</t>
+    <t xml:space="preserve">H-cell</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007237</t>
@@ -3671,7 +3671,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3752,12 +3752,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3890,7 +3884,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4015,10 +4009,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4141,9 +4131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>578880</xdr:colOff>
+      <xdr:colOff>578520</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>131040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4157,8 +4147,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1377720" y="304920"/>
-          <a:ext cx="5925960" cy="1541160"/>
+          <a:off x="1378440" y="304920"/>
+          <a:ext cx="5928480" cy="1540800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4235,10 +4225,10 @@
   <dimension ref="A11:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="F249 J12"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -4418,10 +4408,10 @@
   <dimension ref="A1:J1152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F249 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -7137,10 +7127,10 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="F249 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -8305,11 +8295,11 @@
   </sheetPr>
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F249" activeCellId="0" sqref="F249"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B224" activeCellId="0" sqref="B224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -13540,7 +13530,7 @@
       <c r="A247" s="0" t="s">
         <v>948</v>
       </c>
-      <c r="B247" s="31" t="s">
+      <c r="B247" s="29" t="s">
         <v>949</v>
       </c>
       <c r="C247" s="0" t="s">
@@ -13557,7 +13547,7 @@
       <c r="A248" s="0" t="s">
         <v>951</v>
       </c>
-      <c r="B248" s="31" t="s">
+      <c r="B248" s="29" t="s">
         <v>952</v>
       </c>
       <c r="C248" s="0" t="s">
@@ -13574,7 +13564,7 @@
       <c r="A249" s="0" t="s">
         <v>954</v>
       </c>
-      <c r="B249" s="31" t="s">
+      <c r="B249" s="29" t="s">
         <v>955</v>
       </c>
       <c r="C249" s="0" t="s">
@@ -13594,7 +13584,7 @@
       <c r="A250" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="B250" s="31" t="s">
+      <c r="B250" s="29" t="s">
         <v>958</v>
       </c>
       <c r="C250" s="0" t="s">
@@ -13610,14 +13600,14 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId2" display="https://www.w3.org/TR/2010/NOTE-curie-20101216/"/>
-    <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218, https://w3id.org/nfdi4cat/voc4cat_0007219"/>
+    <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007218"/>
     <hyperlink ref="G211" r:id="rId4" display="https://w3id.org/nfdi4cat/voc4cat_0007259"/>
     <hyperlink ref="A213" r:id="rId5" display="https://w3id.org/nfdi4cat/voc4cat_0007222"/>
     <hyperlink ref="G228" r:id="rId6" display="https://w3id.org/nfdi4cat/voc4cat_0007211, https://w3id.org/nfdi4cat/voc4cat_0000082"/>
     <hyperlink ref="G230" r:id="rId7" display="https://w3id.org/nfdi4cat/voc4cat_0007241, https://w3id.org/nfdi4cat/voc4cat_0007242"/>
     <hyperlink ref="A239" r:id="rId8" display="https://w3id.org/nfdi4cat/voc4cat_0007248"/>
     <hyperlink ref="A240" r:id="rId9" display="https://w3id.org/nfdi4cat/voc4cat_0007249"/>
-    <hyperlink ref="G240" r:id="rId10" display="https://w3id.org/nfdi4cat/voc4cat_0007257"/>
+    <hyperlink ref="G240" r:id="rId10" display="https://w3id.org/nfdi4cat/voc4cat_0007256, https://w3id.org/nfdi4cat/voc4cat_0007257"/>
     <hyperlink ref="A241" r:id="rId11" display="https://w3id.org/nfdi4cat/voc4cat_0007250"/>
     <hyperlink ref="G241" r:id="rId12" display="https://w3id.org/nfdi4cat/voc4cat_0007205, https://w3id.org/nfdi4cat/voc4cat_0007231, https://w3id.org/nfdi4cat/voc4cat_0007232, https://w3id.org/nfdi4cat/voc4cat_0007235, https://w3id.org/nfdi4cat/voc4cat_0007248, https://w3id.org/nfdi4cat/voc4cat_0007236"/>
     <hyperlink ref="A242" r:id="rId13" display="https://w3id.org/nfdi4cat/voc4cat_0007251"/>
@@ -13652,10 +13642,10 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="F249 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -14948,10 +14938,10 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="F249 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -15150,10 +15140,10 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F249 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>

</xml_diff>

<commit_message>
rename dpotential to electrical potential in descriptions, rename number of voltammetry cycles
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="1041">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -2782,7 +2782,7 @@
     <t xml:space="preserve">lower limit potential</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimal potential in a cyclic voltammetry. This is where the sweep turns.</t>
+    <t xml:space="preserve">The minimal electrical potential in a cyclic voltammetry. This is where the sweep turns.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007215</t>
@@ -2791,7 +2791,7 @@
     <t xml:space="preserve">upper limit potential</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximal potential in a cyclic voltammetry. This is where the sweep turns.</t>
+    <t xml:space="preserve">The maximal electrical potential in a cyclic voltammetry. This is where the sweep turns.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007216</t>
@@ -2800,7 +2800,7 @@
     <t xml:space="preserve">initial potential</t>
   </si>
   <si>
-    <t xml:space="preserve">The potential at which a linear sweep or cyclic voltammetry starts.</t>
+    <t xml:space="preserve">The electrical potential at which a linear sweep or cyclic voltammetry starts.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007217</t>
@@ -2809,7 +2809,7 @@
     <t xml:space="preserve">final potential</t>
   </si>
   <si>
-    <t xml:space="preserve">The potential at which a linear sweep or cyclic voltammetry ends.</t>
+    <t xml:space="preserve">The electrical potential at which a linear sweep or cyclic voltammetry ends.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007218</t>
@@ -2818,18 +2818,21 @@
     <t xml:space="preserve">step size potential</t>
   </si>
   <si>
-    <t xml:space="preserve">The potential difference at which the potential in a linear sweep or cyclic voltammetry is altered.</t>
+    <t xml:space="preserve">The electrical potential difference at which the potential in a linear sweep or cyclic voltammetry is altered.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007219</t>
   </si>
   <si>
-    <t xml:space="preserve">electric potential</t>
+    <t xml:space="preserve">electrical potential</t>
   </si>
   <si>
     <t xml:space="preserve">The electrical potential difference between two points in a circuit is the cause of the flow of a current.</t>
   </si>
   <si>
+    <t xml:space="preserve">voltage</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218</t>
   </si>
   <si>
@@ -2911,7 +2914,7 @@
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007228</t>
   </si>
   <si>
-    <t xml:space="preserve">number of cycles</t>
+    <t xml:space="preserve">number of voltammetry cycles</t>
   </si>
   <si>
     <t xml:space="preserve">The number of cycles in a measurement, such as a cyclic voltammetry.</t>
@@ -4131,9 +4134,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>578520</xdr:colOff>
+      <xdr:colOff>578160</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4147,8 +4150,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1378440" y="304920"/>
-          <a:ext cx="5928480" cy="1540800"/>
+          <a:off x="1379160" y="304920"/>
+          <a:ext cx="5931360" cy="1540440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4228,7 +4231,7 @@
       <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -4411,7 +4414,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -7130,7 +7133,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -8295,11 +8298,11 @@
   </sheetPr>
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A183" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D223" activeCellId="0" sqref="D223"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A198" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D205" activeCellId="0" sqref="D205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -12855,7 +12858,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
         <v>825</v>
       </c>
@@ -12868,8 +12871,11 @@
       <c r="D210" s="0" t="s">
         <v>827</v>
       </c>
+      <c r="F210" s="0" t="s">
+        <v>828</v>
+      </c>
       <c r="G210" s="0" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H210" s="0" t="s">
         <v>764</v>
@@ -12877,19 +12883,19 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C211" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="G211" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H211" s="0" t="s">
         <v>764</v>
@@ -12897,16 +12903,16 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C212" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="H212" s="0" t="s">
         <v>764</v>
@@ -12914,16 +12920,16 @@
     </row>
     <row r="213" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C213" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="H213" s="0" t="s">
         <v>764</v>
@@ -12931,16 +12937,16 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C214" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="H214" s="0" t="s">
         <v>764</v>
@@ -12948,16 +12954,16 @@
     </row>
     <row r="215" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C215" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D215" s="28" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H215" s="0" t="s">
         <v>764</v>
@@ -12965,16 +12971,16 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="H216" s="0" t="s">
         <v>764</v>
@@ -12982,16 +12988,16 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="H217" s="0" t="s">
         <v>764</v>
@@ -12999,16 +13005,16 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C218" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="H218" s="0" t="s">
         <v>764</v>
@@ -13016,16 +13022,16 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="H219" s="0" t="s">
         <v>764</v>
@@ -13033,16 +13039,16 @@
     </row>
     <row r="220" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D220" s="28" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="H220" s="0" t="s">
         <v>764</v>
@@ -13050,16 +13056,16 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C221" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="H221" s="0" t="s">
         <v>764</v>
@@ -13067,19 +13073,19 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C222" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="F222" s="0" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="G222" s="29"/>
       <c r="H222" s="0" t="s">
@@ -13088,16 +13094,16 @@
     </row>
     <row r="223" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D223" s="28" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="G223" s="29"/>
       <c r="H223" s="0" t="s">
@@ -13106,16 +13112,16 @@
     </row>
     <row r="224" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D224" s="28" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G224" s="29"/>
       <c r="H224" s="0" t="s">
@@ -13124,16 +13130,16 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="H225" s="0" t="s">
         <v>764</v>
@@ -13141,19 +13147,19 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="F226" s="0" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="G226" s="29"/>
       <c r="H226" s="0" t="s">
@@ -13162,19 +13168,19 @@
     </row>
     <row r="227" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D227" s="28" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="F227" s="0" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="G227" s="29"/>
       <c r="H227" s="0" t="s">
@@ -13183,19 +13189,19 @@
     </row>
     <row r="228" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D228" s="28" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="G228" s="0" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="H228" s="0" t="s">
         <v>764</v>
@@ -13203,16 +13209,16 @@
     </row>
     <row r="229" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D229" s="30" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="H229" s="0" t="s">
         <v>764</v>
@@ -13220,19 +13226,19 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D230" s="0" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="G230" s="0" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="H230" s="0" t="s">
         <v>764</v>
@@ -13240,16 +13246,16 @@
     </row>
     <row r="231" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D231" s="28" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="H231" s="0" t="s">
         <v>764</v>
@@ -13257,16 +13263,16 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D232" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H232" s="0" t="s">
         <v>764</v>
@@ -13274,16 +13280,16 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D233" s="0" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H233" s="0" t="s">
         <v>764</v>
@@ -13291,19 +13297,19 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D234" s="0" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="F234" s="0" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="H234" s="0" t="s">
         <v>764</v>
@@ -13311,16 +13317,16 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D235" s="0" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="H235" s="0" t="s">
         <v>764</v>
@@ -13328,16 +13334,16 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D236" s="0" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="H236" s="0" t="s">
         <v>764</v>
@@ -13345,16 +13351,16 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D237" s="0" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="H237" s="0" t="s">
         <v>764</v>
@@ -13362,16 +13368,16 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C238" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D238" s="0" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="H238" s="0" t="s">
         <v>764</v>
@@ -13379,19 +13385,19 @@
     </row>
     <row r="239" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C239" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D239" s="28" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="F239" s="0" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="G239" s="29"/>
       <c r="H239" s="0" t="s">
@@ -13400,19 +13406,19 @@
     </row>
     <row r="240" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C240" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D240" s="28" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="G240" s="0" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="H240" s="0" t="s">
         <v>764</v>
@@ -13420,19 +13426,19 @@
     </row>
     <row r="241" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C241" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D241" s="0" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="G241" s="29" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="H241" s="0" t="s">
         <v>764</v>
@@ -13440,19 +13446,19 @@
     </row>
     <row r="242" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C242" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D242" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="F242" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="H242" s="0" t="s">
         <v>764</v>
@@ -13460,16 +13466,16 @@
     </row>
     <row r="243" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C243" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D243" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="H243" s="0" t="s">
         <v>764</v>
@@ -13477,16 +13483,16 @@
     </row>
     <row r="244" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C244" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="H244" s="0" t="s">
         <v>764</v>
@@ -13494,16 +13500,16 @@
     </row>
     <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D245" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="H245" s="0" t="s">
         <v>764</v>
@@ -13511,16 +13517,16 @@
     </row>
     <row r="246" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C246" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D246" s="0" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="H246" s="0" t="s">
         <v>764</v>
@@ -13528,16 +13534,16 @@
     </row>
     <row r="247" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C247" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D247" s="28" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="H247" s="0" t="s">
         <v>764</v>
@@ -13545,16 +13551,16 @@
     </row>
     <row r="248" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C248" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D248" s="28" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="H248" s="0" t="s">
         <v>764</v>
@@ -13562,19 +13568,19 @@
     </row>
     <row r="249" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B249" s="29" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C249" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D249" s="28" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="F249" s="0" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="H249" s="0" t="s">
         <v>764</v>
@@ -13582,16 +13588,16 @@
     </row>
     <row r="250" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B250" s="29" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C250" s="0" t="s">
         <v>84</v>
       </c>
       <c r="D250" s="28" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="H250" s="0" t="s">
         <v>764</v>
@@ -13600,7 +13606,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId2" display="https://www.w3.org/TR/2010/NOTE-curie-20101216/"/>
-    <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007218"/>
+    <hyperlink ref="G210" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_0007213, https://w3id.org/nfdi4cat/voc4cat_0007214, https://w3id.org/nfdi4cat/voc4cat_0007215, https://w3id.org/nfdi4cat/voc4cat_0007216, https://w3id.org/nfdi4cat/voc4cat_0007217, https://w3id.org/nfdi4cat/voc4cat_0007218"/>
     <hyperlink ref="G211" r:id="rId4" display="https://w3id.org/nfdi4cat/voc4cat_0007259"/>
     <hyperlink ref="A213" r:id="rId5" display="https://w3id.org/nfdi4cat/voc4cat_0007222"/>
     <hyperlink ref="G228" r:id="rId6" display="https://w3id.org/nfdi4cat/voc4cat_0007211, https://w3id.org/nfdi4cat/voc4cat_0000082"/>
@@ -13645,7 +13651,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -13653,7 +13659,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13661,19 +13667,19 @@
         <v>74</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14941,7 +14947,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -14952,38 +14958,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>120</v>
@@ -14991,16 +14997,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>120</v>
@@ -15143,249 +15149,249 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed terms pa, rt, and extended defintion RT
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -3329,16 +3329,16 @@
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007260</t>
   </si>
   <si>
-    <t xml:space="preserve">retention time gas chromography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A measure of the time taken for a solute to pass through a chromatography column.</t>
+    <t xml:space="preserve">retention time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A measure of the time taken for a solute to pass through a chromatography column. It is the mean of the residence time distribution; it is known as the first moment of the residence time distribution.</t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007261</t>
   </si>
   <si>
-    <t xml:space="preserve">peak area gas chromotography</t>
+    <t xml:space="preserve">peak area</t>
   </si>
   <si>
     <t xml:space="preserve">A measure which is proportional to the amount of a product with a specific retention time. After calibration it is used to calculate gas concentrations of products of an chemical experiment.</t>
@@ -4262,9 +4262,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>580680</xdr:colOff>
+      <xdr:colOff>580320</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4278,8 +4278,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1374480" y="304920"/>
-          <a:ext cx="5911920" cy="1542960"/>
+          <a:off x="1375200" y="304920"/>
+          <a:ext cx="5914440" cy="1542600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4356,10 +4356,10 @@
   <dimension ref="A11:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="H258:H261 J12"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -4539,10 +4539,10 @@
   <dimension ref="A1:J1152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H258:H261 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -7258,10 +7258,10 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="H258:H261 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -8426,11 +8426,11 @@
   </sheetPr>
   <dimension ref="A1:I263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H258" activeCellId="0" sqref="H258:H261"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B258" activeCellId="0" sqref="B258"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -8440,7 +8440,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14051,7 +14051,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
         <v>985</v>
       </c>
@@ -14151,10 +14151,10 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H258:H261 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -15720,16 +15720,16 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H258:H261 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15922,10 +15922,10 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="H258:H261 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>

</xml_diff>

<commit_message>
changed definition of plugflow and fixed typos
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -4099,9 +4099,6 @@
     <t>https://w3id.org/nfdi4cat/voc4cat_0007101</t>
   </si>
   <si>
-    <t xml:space="preserve">Chemical reactors are often claasified by archtype reactors, which can them be extended which multiple divices and so on. The reactor type characterises the basic behavior of a reactor and thus creates a level of comparability. </t>
-  </si>
-  <si>
     <t>https://w3id.org/nfdi4cat/voc4cat_0007102</t>
   </si>
   <si>
@@ -4123,15 +4120,9 @@
     <t>plug flow reactor</t>
   </si>
   <si>
-    <t>An archtype/ideal reactor type, in which a fluid is flowing through the pipe in a plug like manner. A reaction thus takes place over a certain distance in the reactor.</t>
-  </si>
-  <si>
     <t>stirred tank reactor</t>
   </si>
   <si>
-    <t xml:space="preserve">An archtype/ideal reactor type, in which a large volume of fluid is considered to be perfectly mixed and has a certain residence time. Thus contrasting to the plug flow reactor, the reaction does not take place over a certain distance but rather a certain time. </t>
-  </si>
-  <si>
     <t>tubular reactor</t>
   </si>
   <si>
@@ -4157,6 +4148,15 @@
   </si>
   <si>
     <t>0000-0001-5886-7860 Hendrik Borgelt created this resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An abstract concept/ideal reactor type, in which a large volume of fluid is considered to be perfectly mixed and has a certain residence time. Thus contrasting to the plug flow reactor, the reaction does not take place over a certain distance but rather a certain time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical reactors are often classified by abstract concept reactors, which can then be extended with multiple devices and so on. The reactor type characterizes the basic behavior of a reactor and thus creates a level of comparability. </t>
+  </si>
+  <si>
+    <t>An abstract concept/ideal reactor type in which a liquid flows uniformly through the tube, resulting in a straight wave/flow front. A reaction thus takes place over a certain distance in the reactor.</t>
   </si>
 </sst>
 </file>
@@ -9037,8 +9037,8 @@
   </sheetPr>
   <dimension ref="A1:I299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E273" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H295" sqref="H295"/>
+    <sheetView tabSelected="1" topLeftCell="A273" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D300" sqref="D300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15342,133 +15342,133 @@
         <v>84</v>
       </c>
       <c r="D289" t="s">
-        <v>1174</v>
+        <v>1192</v>
       </c>
       <c r="E289" t="s">
         <v>84</v>
       </c>
       <c r="H289" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="13" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B290" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C290" t="s">
         <v>84</v>
       </c>
       <c r="D290" t="s">
-        <v>1182</v>
+        <v>1193</v>
       </c>
       <c r="E290" t="s">
         <v>84</v>
       </c>
       <c r="H290" s="27" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="13" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B291" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C291" t="s">
         <v>84</v>
       </c>
       <c r="D291" t="s">
-        <v>1184</v>
+        <v>1191</v>
       </c>
       <c r="E291" t="s">
         <v>84</v>
       </c>
       <c r="H291" s="27" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="13" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B292" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="C292" t="s">
         <v>84</v>
       </c>
       <c r="D292" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="E292" t="s">
         <v>84</v>
       </c>
       <c r="H292" s="27" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="13" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B293" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="C293" t="s">
         <v>84</v>
       </c>
       <c r="D293" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="E293" t="s">
         <v>84</v>
       </c>
       <c r="H293" s="27" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="13" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B294" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="C294" t="s">
         <v>84</v>
       </c>
       <c r="D294" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="E294" t="s">
         <v>84</v>
       </c>
       <c r="H294" s="27" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="13" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B295" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C295" t="s">
+        <v>84</v>
+      </c>
+      <c r="D295" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E295" t="s">
+        <v>84</v>
+      </c>
+      <c r="H295" s="27" t="s">
         <v>1190</v>
-      </c>
-      <c r="C295" t="s">
-        <v>84</v>
-      </c>
-      <c r="D295" t="s">
-        <v>1192</v>
-      </c>
-      <c r="E295" t="s">
-        <v>84</v>
-      </c>
-      <c r="H295" s="27" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added is are lation to potentiometries
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -686,7 +686,7 @@
     <t xml:space="preserve">An electroanalytical technique based on the measurement of the electromotive force of an electrochemical cell comprised of a measuring and a reference electrode.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007237, htthttps://w3id.org/nfdi4cat/voc4cat_0007208 ps://w3id.org/nfdi4cat/voc4cat_0007212, https://w3id.org/nfdi4cat/voc4cat_0007209 </t>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007237, https://w3id.org/nfdi4cat/voc4cat_0007208, https://w3id.org/nfdi4cat/voc4cat_0007212, https://w3id.org/nfdi4cat/voc4cat_0007209 </t>
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_0007207</t>
@@ -8724,8 +8724,8 @@
   </sheetPr>
   <dimension ref="A1:I288"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G232" activeCellId="0" sqref="G232"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixes typo in original PR
There was a full stop instead of comma in one of the children (column G). Hopefully this solves the error.
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srv-smb3\home$\nmoust\Desktop\Office-PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC810A69-691B-4B9E-A740-132092F1FA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A70941-C860-4080-BA30-28FA7AC6E2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -4983,34 +4983,6 @@
 voc4cat:0007247 (solute), voc4cat:0000199, voc4cat:0000200, voc4cat:0000201</t>
   </si>
   <si>
-    <t>voc4cat:0000001 (photocatalysis),
-voc4cat:0000014 (modification technique),
-voc4cat:0000020 (deposition technique),
-voc4cat:0000045 (synthesis),
-voc4cat:0000049 (synthesis procedure),
-voc4cat:0000066 (characterization technique),
-voc4cat:0000087 (photocatalytic process),
-voc4cat:0000099 (photocatalytic CO2 reduction),
-voc4cat:0000100 (photocatalytic experiment),
-voc4cat:0000123 (blank experiment),
-voc4cat:0000130 (gas chromatography),
-voc4cat:0000137 (mass spectrometry),
-voc4cat:0000141 (liquid chromatography),
-voc4cat:0007001 (heterogeneous catalysis),
-voc4cat:0007002 (thermal catalysis),
-voc4cat:0007029 (hydrothermal synthesis),
-voc4cat:0007031 (flame spray pyrolysis),
-voc4cat:0007206 (potentiometry),
-voc4cat:0007238 (voltammogramm), voc4cat:0000202, voc4cat:0000203, voc4cat:0000204, voc4cat:0000205, voc4cat:0000206, voc4cat:0000207, voc4cat:0000208,</t>
-  </si>
-  <si>
-    <t>voc4cat:0000003 (semiconductor),
-voc4cat:0000005 (metal oxide),
-voc4cat:0000024 (substrate),
-voc4cat:0000194 (catalyst),
-voc4cat:0005056 (material sample), voc4cat:0000196, voc4cat:0000197, voc4cat:0000198. voc4cat:0000210</t>
-  </si>
-  <si>
     <t>voc4cat:0000061 (synthesis equipment),
 voc4cat:0000146 (pressure controller),
 voc4cat:0000151 (temperature controller),
@@ -5188,6 +5160,34 @@
   </si>
   <si>
     <t>https://w3id.org/nfdi4cat/voc4cat_0000195</t>
+  </si>
+  <si>
+    <t>voc4cat:0000003 (semiconductor),
+voc4cat:0000005 (metal oxide),
+voc4cat:0000024 (substrate),
+voc4cat:0000194 (catalyst),
+voc4cat:0005056 (material sample), voc4cat:0000196, voc4cat:0000197, voc4cat:0000198, voc4cat:0000210</t>
+  </si>
+  <si>
+    <t>voc4cat:0000001 (photocatalysis),
+voc4cat:0000014 (modification technique),
+voc4cat:0000020 (deposition technique),
+voc4cat:0000045 (synthesis),
+voc4cat:0000049 (synthesis procedure),
+voc4cat:0000066 (characterization technique),
+voc4cat:0000087 (photocatalytic process),
+voc4cat:0000099 (photocatalytic CO2 reduction),
+voc4cat:0000100 (photocatalytic experiment),
+voc4cat:0000123 (blank experiment),
+voc4cat:0000130 (gas chromatography),
+voc4cat:0000137 (mass spectrometry),
+voc4cat:0000141 (liquid chromatography),
+voc4cat:0007001 (heterogeneous catalysis),
+voc4cat:0007002 (thermal catalysis),
+voc4cat:0007029 (hydrothermal synthesis),
+voc4cat:0007031 (flame spray pyrolysis),
+voc4cat:0007206 (potentiometry),
+voc4cat:0007238 (voltammogramm), voc4cat:0000202, voc4cat:0000203, voc4cat:0000204, voc4cat:0000205, voc4cat:0000206, voc4cat:0000207, voc4cat:0000208</t>
   </si>
 </sst>
 </file>
@@ -10084,13 +10084,13 @@
   </sheetPr>
   <dimension ref="A1:I385"/>
   <sheetViews>
-    <sheetView topLeftCell="A374" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B387" sqref="B387"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G199" sqref="G199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="69.28515625" style="35" customWidth="1"/>
     <col min="2" max="2" width="39.28515625" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="35" customWidth="1"/>
     <col min="4" max="4" width="50.140625" style="35" customWidth="1"/>
@@ -14522,7 +14522,7 @@
       </c>
       <c r="I185" s="36"/>
     </row>
-    <row r="186" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A186" s="36" t="s">
         <v>1306</v>
       </c>
@@ -14565,7 +14565,7 @@
       </c>
       <c r="F187" s="26"/>
       <c r="G187" s="26" t="s">
-        <v>1464</v>
+        <v>1487</v>
       </c>
       <c r="H187" s="26" t="s">
         <v>1240</v>
@@ -14590,7 +14590,7 @@
       </c>
       <c r="F188" s="26"/>
       <c r="G188" s="26" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="H188" s="26" t="s">
         <v>1240</v>
@@ -14615,7 +14615,7 @@
       </c>
       <c r="F189" s="26"/>
       <c r="G189" s="26" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="H189" s="26" t="s">
         <v>93</v>
@@ -14690,7 +14690,7 @@
       </c>
       <c r="F192" s="26"/>
       <c r="G192" s="26" t="s">
-        <v>1465</v>
+        <v>1486</v>
       </c>
       <c r="H192" s="26" t="s">
         <v>93</v>
@@ -18815,7 +18815,7 @@
     </row>
     <row r="367" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A367" s="25" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="B367" s="22" t="s">
         <v>346</v>
@@ -18835,7 +18835,7 @@
     </row>
     <row r="368" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A368" s="25" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="B368" s="35" t="s">
         <v>1457</v>
@@ -18858,7 +18858,7 @@
     </row>
     <row r="369" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A369" s="25" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B369" s="22" t="s">
         <v>1422</v>
@@ -18878,7 +18878,7 @@
     </row>
     <row r="370" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A370" s="25" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="B370" s="22" t="s">
         <v>357</v>
@@ -18898,7 +18898,7 @@
     </row>
     <row r="371" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A371" s="25" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B371" s="35" t="s">
         <v>1458</v>
@@ -18921,7 +18921,7 @@
     </row>
     <row r="372" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A372" s="25" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="B372" s="35" t="s">
         <v>1423</v>
@@ -18944,7 +18944,7 @@
     </row>
     <row r="373" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A373" s="25" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="B373" s="22" t="s">
         <v>1461</v>
@@ -18967,7 +18967,7 @@
     </row>
     <row r="374" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A374" s="25" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="B374" s="35" t="s">
         <v>1424</v>
@@ -18987,7 +18987,7 @@
     </row>
     <row r="375" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" s="25" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="B375" s="22" t="s">
         <v>1425</v>
@@ -19007,7 +19007,7 @@
     </row>
     <row r="376" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A376" s="25" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="B376" s="35" t="s">
         <v>1426</v>
@@ -19027,7 +19027,7 @@
     </row>
     <row r="377" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A377" s="25" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B377" s="22" t="s">
         <v>1427</v>
@@ -19050,7 +19050,7 @@
     </row>
     <row r="378" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A378" s="25" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="B378" s="22" t="s">
         <v>1428</v>
@@ -19070,7 +19070,7 @@
     </row>
     <row r="379" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A379" s="25" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="B379" s="22" t="s">
         <v>1429</v>
@@ -19090,7 +19090,7 @@
     </row>
     <row r="380" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A380" s="25" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="B380" s="35" t="s">
         <v>1430</v>
@@ -19110,7 +19110,7 @@
     </row>
     <row r="381" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A381" s="25" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="B381" s="35" t="s">
         <v>1431</v>
@@ -19130,7 +19130,7 @@
     </row>
     <row r="382" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A382" s="25" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="B382" s="35" t="s">
         <v>1432</v>
@@ -19150,7 +19150,7 @@
     </row>
     <row r="383" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A383" s="25" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="B383" s="35" t="s">
         <v>1433</v>
@@ -19170,7 +19170,7 @@
     </row>
     <row r="384" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A384" s="25" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="B384" s="22" t="s">
         <v>1434</v>
@@ -19190,7 +19190,7 @@
     </row>
     <row r="385" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A385" s="25" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B385" s="35" t="s">
         <v>1435</v>
@@ -20328,13 +20328,13 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="70.85546875" style="35" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" style="35" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" style="35" customWidth="1"/>
     <col min="4" max="4" width="70.7109375" style="35" customWidth="1"/>
@@ -20399,7 +20399,7 @@
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>1418</v>

</xml_diff>

<commit_message>
Remove attribute children for correct hierarchy
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/voc4cat.xlsx
+++ b/inbox-excel-vocabs/voc4cat.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="1935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3426" uniqueCount="1935">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -5896,7 +5896,6 @@
 voc4cat:0007261 (peak area),
 voc4cat:0007262 (membrane thickness),
 voc4cat:0007263 (total faradaic efficiency),
-voc4cat:0008084 (detector dead time),
 voc4cat:0008085 (dead time correction),
 voc4cat:0008086 (fluorescence yield),
 voc4cat:0008087 (absorbance),
@@ -5904,11 +5903,6 @@
 voc4cat:0008089 (absorbance of the sample),
 voc4cat:0008090 (manual energy shift),
 voc4cat:0008091 (fluorescence signal),
-voc4cat:0008092 (incoming count rate),
-voc4cat:0008093 (outgoing count rate),
-voc4cat:0008094 (trigger live time),
-voc4cat:0008095 (effective measurement time),
-voc4cat:0008096 (total measurement time),
 voc4cat:0008097 (X-ray photon energy),
 voc4cat:0008099 (dead time),
 voc4cat:0008100 (detector performance measure)
@@ -7380,9 +7374,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>579240</xdr:colOff>
+      <xdr:colOff>578520</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>131040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7396,8 +7390,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1377360" y="304920"/>
-          <a:ext cx="5910120" cy="1541520"/>
+          <a:off x="1378440" y="304920"/>
+          <a:ext cx="5909400" cy="1540800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7473,11 +7467,11 @@
   </sheetPr>
   <dimension ref="A11:L32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.28"/>
@@ -7666,11 +7660,11 @@
   </sheetPr>
   <dimension ref="A1:J1149"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16"/>
@@ -10354,11 +10348,11 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.7"/>
@@ -11526,11 +11520,11 @@
   </sheetPr>
   <dimension ref="A1:I527"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B491" activeCellId="0" sqref="B491"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A500" activeCellId="0" sqref="A500"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.7"/>
@@ -22983,7 +22977,7 @@
       </c>
       <c r="I480" s="34"/>
     </row>
-    <row r="481" customFormat="false" ht="1706.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="481" customFormat="false" ht="1624.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="34" t="s">
         <v>1734</v>
       </c>
@@ -23407,7 +23401,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="500" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="500" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="34" t="s">
         <v>1807</v>
       </c>
@@ -23426,6 +23420,9 @@
       <c r="F500" s="0"/>
       <c r="G500" s="35" t="s">
         <v>1810</v>
+      </c>
+      <c r="H500" s="1" t="s">
+        <v>1742</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23940,11 +23937,11 @@
   </sheetPr>
   <dimension ref="A1:F461"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="42.71"/>
   </cols>
@@ -24720,11 +24717,11 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.7"/>
@@ -25003,11 +25000,11 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="60.72"/>

</xml_diff>